<commit_message>
calibrate investment for solar, wind, combined cycle
</commit_message>
<xml_diff>
--- a/data/database/DATA_Enerdata_input ThreeMe.xlsx
+++ b/data/database/DATA_Enerdata_input ThreeMe.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gissela.Landa\Documents\Github\ThreeMe-Mex\data\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Energy final consumption-Mtoe" sheetId="1" r:id="rId1"/>
@@ -66,14 +71,13 @@
     <definedName name="solver_ssz" hidden="1">100</definedName>
     <definedName name="solver_ver" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId10"/>
     <pivotCache cacheId="1" r:id="rId11"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -423,15 +427,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,7 +565,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,6 +617,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -870,16 +880,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -963,7 +973,7 @@
     <xf numFmtId="3" fontId="3" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -987,7 +997,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1000,14 +1010,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1021,10 +1031,10 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -1083,6 +1093,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Milliers 3" xfId="3"/>
@@ -1096,256 +1113,256 @@
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -1372,10 +1389,10 @@
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.0"/>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1696,11 +1713,11 @@
     <worksheetSource ref="B2:J69" sheet="Energy final consumption-PJ"/>
   </cacheSource>
   <cacheFields count="10">
-    <cacheField name="Sector" numFmtId="165">
+    <cacheField name="Sector" numFmtId="164">
       <sharedItems count="6">
         <s v="Agriculture"/>
         <s v="Industries"/>
-        <s v="Transport &#10;"/>
+        <s v="Transport _x000a_"/>
         <s v="Services"/>
         <s v="Energy"/>
         <s v="Household"/>
@@ -2108,11 +2125,11 @@
     <worksheetSource ref="L2:T69" sheet="Energy final consumption-PJ"/>
   </cacheSource>
   <cacheFields count="10">
-    <cacheField name="Sector" numFmtId="165">
+    <cacheField name="Sector" numFmtId="164">
       <sharedItems count="6">
         <s v="Agriculture"/>
         <s v="Industries"/>
-        <s v="Transport &#10;"/>
+        <s v="Transport _x000a_"/>
         <s v="Services"/>
         <s v="Energy"/>
         <s v="Household"/>
@@ -5957,21 +5974,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
@@ -5984,7 +6001,7 @@
     <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>74</v>
       </c>
@@ -6009,7 +6026,7 @@
       <c r="S1" s="89"/>
       <c r="T1" s="90"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>71</v>
       </c>
@@ -6066,7 +6083,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="14.45" customHeight="1">
+    <row r="3" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="57" t="s">
         <v>50</v>
@@ -6124,7 +6141,7 @@
         <v>2.4266706759312591</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="57" t="s">
         <v>50</v>
@@ -6182,7 +6199,7 @@
         <v>0.86391552164465646</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="14.45" customHeight="1">
+    <row r="5" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="58" t="s">
         <v>53</v>
@@ -6240,7 +6257,7 @@
         <v>0.13265023384801955</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="14.45" customHeight="1">
+    <row r="6" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="58" t="s">
         <v>53</v>
@@ -6298,7 +6315,7 @@
         <v>0.40459703937524383</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="14.45" customHeight="1">
+    <row r="7" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="58" t="s">
         <v>53</v>
@@ -6356,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="14.45" customHeight="1">
+    <row r="8" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="58" t="s">
         <v>53</v>
@@ -6414,7 +6431,7 @@
         <v>0.25765293416535168</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="14.45" customHeight="1">
+    <row r="9" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="58" t="s">
         <v>53</v>
@@ -6472,7 +6489,7 @@
         <v>0.91468653057259042</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.45" customHeight="1">
+    <row r="10" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="58" t="s">
         <v>53</v>
@@ -6530,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="14.45" customHeight="1">
+    <row r="11" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="58" t="s">
         <v>53</v>
@@ -6588,7 +6605,7 @@
         <v>1.2678098357632004</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="14.45" customHeight="1">
+    <row r="12" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="58" t="s">
         <v>53</v>
@@ -6646,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.45" customHeight="1">
+    <row r="13" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="58" t="s">
         <v>53</v>
@@ -6704,7 +6721,7 @@
         <v>0.51091916083968003</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="14.45" customHeight="1">
+    <row r="14" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="58" t="s">
         <v>53</v>
@@ -6762,7 +6779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.45" customHeight="1">
+    <row r="15" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="58" t="s">
         <v>53</v>
@@ -6820,7 +6837,7 @@
         <v>6.2414144996665852E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.45" customHeight="1">
+    <row r="16" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="58" t="s">
         <v>53</v>
@@ -6878,7 +6895,7 @@
         <v>3.9943296971200137</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="14.45" customHeight="1">
+    <row r="17" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="58" t="s">
         <v>53</v>
@@ -6936,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="14.45" customHeight="1">
+    <row r="18" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="58" t="s">
         <v>53</v>
@@ -6994,7 +7011,7 @@
         <v>0.75475240316940861</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="14.45" customHeight="1">
+    <row r="19" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="58" t="s">
         <v>53</v>
@@ -7052,7 +7069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="14.45" customHeight="1">
+    <row r="20" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="58" t="s">
         <v>53</v>
@@ -7110,7 +7127,7 @@
         <v>3.9551168896105011</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="14.45" customHeight="1">
+    <row r="21" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="58" t="s">
         <v>53</v>
@@ -7168,7 +7185,7 @@
         <v>0.23583974078556555</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14.45" customHeight="1">
+    <row r="22" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="58" t="s">
         <v>53</v>
@@ -7226,7 +7243,7 @@
         <v>0.20939715483683882</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="14.45" customHeight="1">
+    <row r="23" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="58" t="s">
         <v>53</v>
@@ -7284,7 +7301,7 @@
         <v>0.77692205967969596</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="14.45" customHeight="1">
+    <row r="24" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="58" t="s">
         <v>53</v>
@@ -7342,7 +7359,7 @@
         <v>1.3606138891474937</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="14.45" customHeight="1">
+    <row r="25" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="58" t="s">
         <v>53</v>
@@ -7400,7 +7417,7 @@
         <v>6.931392798986015E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="14.45" customHeight="1">
+    <row r="26" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="58" t="s">
         <v>53</v>
@@ -7458,7 +7475,7 @@
         <v>3.2484511258581366</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="14.45" customHeight="1">
+    <row r="27" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="58" t="s">
         <v>53</v>
@@ -7516,7 +7533,7 @@
         <v>1.6454462934439529</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="14.45" customHeight="1">
+    <row r="28" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="58" t="s">
         <v>53</v>
@@ -7574,7 +7591,7 @@
         <v>0.75244039451453226</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="14.45" customHeight="1">
+    <row r="29" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="58" t="s">
         <v>53</v>
@@ -7632,7 +7649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="14.45" customHeight="1">
+    <row r="30" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="58" t="s">
         <v>53</v>
@@ -7690,7 +7707,7 @@
         <v>1.2408380497043639E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="14.45" customHeight="1">
+    <row r="31" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="58" t="s">
         <v>53</v>
@@ -7748,7 +7765,7 @@
         <v>0.22641381854695641</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="14.45" customHeight="1">
+    <row r="32" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="58" t="s">
         <v>53</v>
@@ -7806,7 +7823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="14.45" customHeight="1">
+    <row r="33" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="58" t="s">
         <v>53</v>
@@ -7864,7 +7881,7 @@
         <v>0.49519795111159992</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="14.45" customHeight="1">
+    <row r="34" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="58" t="s">
         <v>53</v>
@@ -7922,7 +7939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="14.45" customHeight="1">
+    <row r="35" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="58" t="s">
         <v>53</v>
@@ -7952,7 +7969,7 @@
       <c r="S35" s="40"/>
       <c r="T35" s="42"/>
     </row>
-    <row r="36" spans="1:20" ht="14.45" customHeight="1">
+    <row r="36" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="58" t="s">
         <v>53</v>
@@ -8010,7 +8027,7 @@
         <v>1.7463287910938832</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="14.45" customHeight="1">
+    <row r="37" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="58" t="s">
         <v>53</v>
@@ -8068,7 +8085,7 @@
         <v>1.9294457929217028</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="14.45" customHeight="1">
+    <row r="38" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="58" t="s">
         <v>53</v>
@@ -8126,7 +8143,7 @@
         <v>0.8327853913974711</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="14.45" customHeight="1">
+    <row r="39" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="58" t="s">
         <v>53</v>
@@ -8184,7 +8201,7 @@
         <v>11.276026452721876</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="14.45" customHeight="1">
+    <row r="40" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
       <c r="B40" s="58" t="s">
         <v>53</v>
@@ -8242,7 +8259,7 @@
         <v>0.93901644264645512</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="14.45" customHeight="1">
+    <row r="41" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="58" t="s">
         <v>53</v>
@@ -8300,7 +8317,7 @@
         <v>14.50246197122239</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="15" customHeight="1">
+    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
       <c r="B42" s="58" t="s">
         <v>53</v>
@@ -8358,7 +8375,7 @@
         <v>0.22882670570777064</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="17.25" customHeight="1">
+    <row r="43" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="51" t="s">
         <v>12</v>
@@ -8416,7 +8433,7 @@
         <v>9.9442889884905004</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="14.45" customHeight="1">
+    <row r="44" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="51" t="s">
         <v>12</v>
@@ -8474,7 +8491,7 @@
         <v>0.59973686076159449</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="14.45" customHeight="1">
+    <row r="45" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="51" t="s">
         <v>12</v>
@@ -8532,7 +8549,7 @@
         <v>0.76306309361341929</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="15.75" customHeight="1">
+    <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="51" t="s">
         <v>12</v>
@@ -8590,7 +8607,7 @@
         <v>1.3935023160563289</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="14.45" customHeight="1">
+    <row r="47" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="51" t="s">
         <v>12</v>
@@ -8648,7 +8665,7 @@
         <v>17.713605950448237</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="14.45" customHeight="1">
+    <row r="48" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
       <c r="B48" s="51" t="s">
         <v>12</v>
@@ -8706,7 +8723,7 @@
         <v>1.358943230442103</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="14.45" customHeight="1">
+    <row r="49" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="51" t="s">
         <v>12</v>
@@ -8764,7 +8781,7 @@
         <v>2.5185190564531243</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="14.45" customHeight="1">
+    <row r="50" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="51" t="s">
         <v>12</v>
@@ -8822,7 +8839,7 @@
         <v>1.3134376181723597</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="14.45" customHeight="1">
+    <row r="51" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="51" t="s">
         <v>12</v>
@@ -8880,7 +8897,7 @@
         <v>0.12153340884723349</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="15" customHeight="1">
+    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="51" t="s">
         <v>12</v>
@@ -8910,7 +8927,7 @@
       <c r="S52" s="40"/>
       <c r="T52" s="42"/>
     </row>
-    <row r="53" spans="1:20" ht="14.45" customHeight="1">
+    <row r="53" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
       <c r="B53" s="58" t="s">
         <v>46</v>
@@ -8968,7 +8985,7 @@
         <v>0.9633155727291447</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="14.45" customHeight="1">
+    <row r="54" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="58" t="s">
         <v>46</v>
@@ -9026,7 +9043,7 @@
         <v>0.49959607856781713</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="14.45" customHeight="1">
+    <row r="55" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="58" t="s">
         <v>46</v>
@@ -9084,7 +9101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="14.45" customHeight="1">
+    <row r="56" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="58" t="s">
         <v>46</v>
@@ -9142,7 +9159,7 @@
         <v>1.1475449889419003</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="14.45" customHeight="1">
+    <row r="57" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="58" t="s">
         <v>46</v>
@@ -9200,7 +9217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="15" customHeight="1">
+    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
       <c r="B58" s="58" t="s">
         <v>46</v>
@@ -9258,7 +9275,7 @@
         <v>0.17310716792572445</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="14.25" customHeight="1">
+    <row r="59" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="58" t="s">
         <v>49</v>
@@ -9288,7 +9305,7 @@
       <c r="S59" s="43"/>
       <c r="T59" s="43"/>
     </row>
-    <row r="60" spans="1:20" ht="14.45" customHeight="1">
+    <row r="60" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="58" t="s">
         <v>49</v>
@@ -9318,7 +9335,7 @@
       <c r="S60" s="43"/>
       <c r="T60" s="43"/>
     </row>
-    <row r="61" spans="1:20" ht="14.45" customHeight="1">
+    <row r="61" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
       <c r="B61" s="58" t="s">
         <v>49</v>
@@ -9348,7 +9365,7 @@
       <c r="S61" s="43"/>
       <c r="T61" s="43"/>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
       <c r="B62" s="59" t="s">
         <v>62</v>
@@ -9406,7 +9423,7 @@
         <v>6.5972259617426188</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="59" t="s">
         <v>62</v>
@@ -9464,7 +9481,7 @@
         <v>1.5871293117384999</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
       <c r="B64" s="59" t="s">
         <v>62</v>
@@ -9522,7 +9539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
       <c r="B65" s="59" t="s">
         <v>62</v>
@@ -9580,7 +9597,7 @@
         <v>6.5572353395536576</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
       <c r="B66" s="59" t="s">
         <v>62</v>
@@ -9638,7 +9655,7 @@
         <v>1.7835081250084326</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
       <c r="B67" s="59" t="s">
         <v>62</v>
@@ -9696,7 +9713,7 @@
         <v>1.2607923527182634</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="12.95" customHeight="1">
+    <row r="68" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="59" t="s">
         <v>62</v>
       </c>
@@ -9753,7 +9770,7 @@
         <v>16.294795036187946</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="12.95" customHeight="1">
+    <row r="69" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="59" t="s">
         <v>62</v>
       </c>
@@ -9810,7 +9827,7 @@
         <v>2.2721832151407417</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C70" s="2" t="s">
         <v>1</v>
       </c>
@@ -9869,7 +9886,7 @@
         <v>36.352869342090159</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C71" s="7" t="s">
         <v>0</v>
       </c>
@@ -9928,7 +9945,7 @@
         <v>130.89591502469946</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C72" s="7"/>
       <c r="D72" s="19"/>
       <c r="E72" s="18"/>
@@ -9937,7 +9954,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="16"/>
     </row>
-    <row r="73" spans="1:20" ht="15">
+    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="C73" s="13"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
@@ -9945,7 +9962,7 @@
       <c r="H73" s="15"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
@@ -9953,18 +9970,18 @@
       <c r="H74" s="10"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H75" s="10"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H76" s="10"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="1:20" ht="15">
+    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
       <c r="C78" s="13"/>
@@ -9974,7 +9991,7 @@
       <c r="G78" s="11"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -9984,7 +10001,7 @@
       <c r="G79" s="8"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="7"/>
@@ -9994,7 +10011,7 @@
       <c r="G80" s="6"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="7"/>
@@ -10004,7 +10021,7 @@
       <c r="G81" s="6"/>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="7"/>
@@ -10014,7 +10031,7 @@
       <c r="G82" s="6"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="7"/>
@@ -10024,7 +10041,7 @@
       <c r="G83" s="6"/>
       <c r="I83" s="4"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="7"/>
@@ -10034,7 +10051,7 @@
       <c r="G84" s="6"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="7"/>
@@ -10044,7 +10061,7 @@
       <c r="G85" s="6"/>
       <c r="I85" s="4"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="7"/>
@@ -10054,7 +10071,7 @@
       <c r="G86" s="6"/>
       <c r="I86" s="4"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="7"/>
@@ -10064,7 +10081,7 @@
       <c r="G87" s="6"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="7"/>
@@ -10074,7 +10091,7 @@
       <c r="G88" s="6"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="7"/>
@@ -10084,7 +10101,7 @@
       <c r="G89" s="6"/>
       <c r="I89" s="4"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="7"/>
@@ -10094,7 +10111,7 @@
       <c r="G90" s="6"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="7"/>
@@ -10104,7 +10121,7 @@
       <c r="G91" s="6"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="7"/>
@@ -10114,7 +10131,7 @@
       <c r="G92" s="6"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="7"/>
@@ -10124,7 +10141,7 @@
       <c r="G93" s="6"/>
       <c r="I93" s="4"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="7"/>
@@ -10134,7 +10151,7 @@
       <c r="G94" s="6"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="7"/>
@@ -10144,7 +10161,7 @@
       <c r="G95" s="6"/>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="7"/>
@@ -10154,7 +10171,7 @@
       <c r="G96" s="6"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="7"/>
@@ -10164,7 +10181,7 @@
       <c r="G97" s="6"/>
       <c r="I97" s="4"/>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="7"/>
@@ -10174,7 +10191,7 @@
       <c r="G98" s="6"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="7"/>
@@ -10184,7 +10201,7 @@
       <c r="G99" s="6"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="7"/>
@@ -10194,7 +10211,7 @@
       <c r="G100" s="6"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="7"/>
@@ -10203,7 +10220,7 @@
       <c r="F101" s="6"/>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="7"/>
@@ -10212,7 +10229,7 @@
       <c r="F102" s="6"/>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="7"/>
@@ -10221,7 +10238,7 @@
       <c r="F103" s="6"/>
       <c r="I103" s="4"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="7"/>
@@ -10230,7 +10247,7 @@
       <c r="F104" s="6"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="7"/>
@@ -10239,7 +10256,7 @@
       <c r="F105" s="6"/>
       <c r="I105" s="4"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="5"/>
       <c r="B106" s="5"/>
       <c r="C106" s="7"/>
@@ -10248,7 +10265,7 @@
       <c r="F106" s="6"/>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="7"/>
@@ -10257,7 +10274,7 @@
       <c r="F107" s="6"/>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
       <c r="C108" s="7"/>
@@ -10266,7 +10283,7 @@
       <c r="F108" s="6"/>
       <c r="I108" s="4"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="7"/>
@@ -10275,7 +10292,7 @@
       <c r="F109" s="6"/>
       <c r="I109" s="4"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
       <c r="C110" s="7"/>
@@ -10284,7 +10301,7 @@
       <c r="F110" s="6"/>
       <c r="I110" s="4"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="7"/>
@@ -10293,37 +10310,37 @@
       <c r="F111" s="6"/>
       <c r="I111" s="4"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
       <c r="D112" s="2"/>
       <c r="I112" s="4"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="2"/>
@@ -10416,14 +10433,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T117"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
@@ -10436,7 +10453,7 @@
     <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>74</v>
       </c>
@@ -10461,7 +10478,7 @@
       <c r="S1" s="89"/>
       <c r="T1" s="90"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>71</v>
       </c>
@@ -10518,7 +10535,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="14.45" customHeight="1">
+    <row r="3" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="57" t="s">
         <v>50</v>
@@ -10588,7 +10605,7 @@
         <v>101.59984785988996</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="57" t="s">
         <v>50</v>
@@ -10658,7 +10675,7 @@
         <v>36.170415060218481</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="14.45" customHeight="1">
+    <row r="5" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="58" t="s">
         <v>53</v>
@@ -10728,7 +10745,7 @@
         <v>5.5537999907488826</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="14.45" customHeight="1">
+    <row r="6" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="58" t="s">
         <v>53</v>
@@ -10798,7 +10815,7 @@
         <v>16.939668844562711</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="14.45" customHeight="1">
+    <row r="7" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="58" t="s">
         <v>53</v>
@@ -10868,7 +10885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="14.45" customHeight="1">
+    <row r="8" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="58" t="s">
         <v>53</v>
@@ -10938,7 +10955,7 @@
         <v>10.787413047634944</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="14.45" customHeight="1">
+    <row r="9" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="58" t="s">
         <v>53</v>
@@ -11008,7 +11025,7 @@
         <v>38.296095662013215</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.45" customHeight="1">
+    <row r="10" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="58" t="s">
         <v>53</v>
@@ -11078,7 +11095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="14.45" customHeight="1">
+    <row r="11" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="58" t="s">
         <v>53</v>
@@ -11148,7 +11165,7 @@
         <v>53.080662203733674</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="14.45" customHeight="1">
+    <row r="12" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="58" t="s">
         <v>53</v>
@@ -11218,7 +11235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.45" customHeight="1">
+    <row r="13" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="58" t="s">
         <v>53</v>
@@ -11288,7 +11305,7 @@
         <v>21.391163426035725</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="14.45" customHeight="1">
+    <row r="14" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="58" t="s">
         <v>53</v>
@@ -11358,7 +11375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.45" customHeight="1">
+    <row r="15" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="58" t="s">
         <v>53</v>
@@ -11428,7 +11445,7 @@
         <v>2.6131554227204061</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.45" customHeight="1">
+    <row r="16" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="58" t="s">
         <v>53</v>
@@ -11498,7 +11515,7 @@
         <v>167.23459575902075</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="14.45" customHeight="1">
+    <row r="17" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="58" t="s">
         <v>53</v>
@@ -11568,7 +11585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="14.45" customHeight="1">
+    <row r="18" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="58" t="s">
         <v>53</v>
@@ -11638,7 +11655,7 @@
         <v>31.599973615896801</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="14.45" customHeight="1">
+    <row r="19" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="58" t="s">
         <v>53</v>
@@ -11708,7 +11725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="14.45" customHeight="1">
+    <row r="20" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="58" t="s">
         <v>53</v>
@@ -11778,7 +11795,7 @@
         <v>165.59283393421248</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="14.45" customHeight="1">
+    <row r="21" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="58" t="s">
         <v>53</v>
@@ -11848,7 +11865,7 @@
         <v>9.8741382672100588</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14.45" customHeight="1">
+    <row r="22" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="58" t="s">
         <v>53</v>
@@ -11918,7 +11935,7 @@
         <v>8.767040078708769</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="14.45" customHeight="1">
+    <row r="23" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="58" t="s">
         <v>53</v>
@@ -11988,7 +12005,7 @@
         <v>32.528172794669516</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="14.45" customHeight="1">
+    <row r="24" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="58" t="s">
         <v>53</v>
@@ -12058,7 +12075,7 @@
         <v>56.966182310827271</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="14.45" customHeight="1">
+    <row r="25" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="58" t="s">
         <v>53</v>
@@ -12128,7 +12145,7 @@
         <v>2.902035537079465</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="14.45" customHeight="1">
+    <row r="26" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="58" t="s">
         <v>53</v>
@@ -12198,7 +12215,7 @@
         <v>136.00615173742847</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="14.45" customHeight="1">
+    <row r="27" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="58" t="s">
         <v>53</v>
@@ -12268,7 +12285,7 @@
         <v>68.891545413911416</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="14.45" customHeight="1">
+    <row r="28" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="58" t="s">
         <v>53</v>
@@ -12338,7 +12355,7 @@
         <v>31.503174437534437</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="14.45" customHeight="1">
+    <row r="29" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="58" t="s">
         <v>53</v>
@@ -12408,7 +12425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="14.45" customHeight="1">
+    <row r="30" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="58" t="s">
         <v>53</v>
@@ -12478,7 +12495,7 @@
         <v>0.51951407465022315</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="14.45" customHeight="1">
+    <row r="31" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="58" t="s">
         <v>53</v>
@@ -12548,7 +12565,7 @@
         <v>9.4794937549239719</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="14.45" customHeight="1">
+    <row r="32" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="58" t="s">
         <v>53</v>
@@ -12618,7 +12635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="14.45" customHeight="1">
+    <row r="33" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="58" t="s">
         <v>53</v>
@@ -12688,7 +12705,7 @@
         <v>20.732947817140467</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="14.45" customHeight="1">
+    <row r="34" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="58" t="s">
         <v>53</v>
@@ -12758,7 +12775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="14.45" customHeight="1">
+    <row r="35" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="58" t="s">
         <v>53</v>
@@ -12788,7 +12805,7 @@
       <c r="S35" s="40"/>
       <c r="T35" s="42"/>
     </row>
-    <row r="36" spans="1:20" ht="14.45" customHeight="1">
+    <row r="36" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="58" t="s">
         <v>53</v>
@@ -12858,7 +12875,7 @@
         <v>73.115293825518705</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="14.45" customHeight="1">
+    <row r="37" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="58" t="s">
         <v>53</v>
@@ -12928,7 +12945,7 @@
         <v>80.782036458045852</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="14.45" customHeight="1">
+    <row r="38" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="58" t="s">
         <v>53</v>
@@ -12998,7 +13015,7 @@
         <v>34.86705876702932</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="14.45" customHeight="1">
+    <row r="39" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="58" t="s">
         <v>53</v>
@@ -13068,7 +13085,7 @@
         <v>472.10467552255955</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="14.45" customHeight="1">
+    <row r="40" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
       <c r="B40" s="58" t="s">
         <v>53</v>
@@ -13138,7 +13155,7 @@
         <v>39.314740420721783</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="14.45" customHeight="1">
+    <row r="41" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="58" t="s">
         <v>53</v>
@@ -13208,7 +13225,7 @@
         <v>607.1890778111391</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="15" customHeight="1">
+    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
       <c r="B42" s="58" t="s">
         <v>53</v>
@@ -13278,7 +13295,7 @@
         <v>9.5805165145729418</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="17.25" customHeight="1">
+    <row r="43" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="51" t="s">
         <v>12</v>
@@ -13348,7 +13365,7 @@
         <v>416.34749137012028</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="14.45" customHeight="1">
+    <row r="44" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="51" t="s">
         <v>12</v>
@@ -13418,7 +13435,7 @@
         <v>25.109782886366439</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="14.45" customHeight="1">
+    <row r="45" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="51" t="s">
         <v>12</v>
@@ -13488,7 +13505,7 @@
         <v>31.947925603406642</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="15.75" customHeight="1">
+    <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="51" t="s">
         <v>12</v>
@@ -13558,7 +13575,7 @@
         <v>58.343154968646381</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="14.45" customHeight="1">
+    <row r="47" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="51" t="s">
         <v>12</v>
@@ -13628,7 +13645,7 @@
         <v>741.63325393336686</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="14.45" customHeight="1">
+    <row r="48" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
       <c r="B48" s="51" t="s">
         <v>12</v>
@@ -13698,7 +13715,7 @@
         <v>56.896235172149972</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="14.45" customHeight="1">
+    <row r="49" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="51" t="s">
         <v>12</v>
@@ -13768,7 +13785,7 @@
         <v>105.44535585557942</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="14.45" customHeight="1">
+    <row r="50" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="51" t="s">
         <v>12</v>
@@ -13838,7 +13855,7 @@
         <v>54.99100619764036</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="14.45" customHeight="1">
+    <row r="51" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="51" t="s">
         <v>12</v>
@@ -13908,7 +13925,7 @@
         <v>5.0883607616159718</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="15" customHeight="1">
+    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="51" t="s">
         <v>12</v>
@@ -13938,7 +13955,7 @@
       <c r="S52" s="40"/>
       <c r="T52" s="42"/>
     </row>
-    <row r="53" spans="1:20" ht="14.45" customHeight="1">
+    <row r="53" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
       <c r="B53" s="58" t="s">
         <v>46</v>
@@ -14008,7 +14025,7 @@
         <v>40.332096399023833</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="14.45" customHeight="1">
+    <row r="54" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="58" t="s">
         <v>46</v>
@@ -14078,7 +14095,7 @@
         <v>20.917088617477368</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="14.45" customHeight="1">
+    <row r="55" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="58" t="s">
         <v>46</v>
@@ -14148,7 +14165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="14.45" customHeight="1">
+    <row r="56" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="58" t="s">
         <v>46</v>
@@ -14218,7 +14235,7 @@
         <v>48.045413597019483</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="14.45" customHeight="1">
+    <row r="57" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="58" t="s">
         <v>46</v>
@@ -14288,7 +14305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="15" customHeight="1">
+    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
       <c r="B58" s="58" t="s">
         <v>46</v>
@@ -14358,7 +14375,7 @@
         <v>7.2476509067142318</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="14.25" customHeight="1">
+    <row r="59" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="58" t="s">
         <v>49</v>
@@ -14388,7 +14405,7 @@
       <c r="S59" s="43"/>
       <c r="T59" s="43"/>
     </row>
-    <row r="60" spans="1:20" ht="14.45" customHeight="1">
+    <row r="60" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="58" t="s">
         <v>49</v>
@@ -14418,7 +14435,7 @@
       <c r="S60" s="43"/>
       <c r="T60" s="43"/>
     </row>
-    <row r="61" spans="1:20" ht="14.45" customHeight="1">
+    <row r="61" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
       <c r="B61" s="58" t="s">
         <v>49</v>
@@ -14448,7 +14465,7 @@
       <c r="S61" s="43"/>
       <c r="T61" s="43"/>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
       <c r="B62" s="59" t="s">
         <v>62</v>
@@ -14518,7 +14535,7 @@
         <v>276.21265656623996</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="59" t="s">
         <v>62</v>
@@ -14588,7 +14605,7 @@
         <v>66.449930023867523</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
       <c r="B64" s="59" t="s">
         <v>62</v>
@@ -14658,7 +14675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
       <c r="B65" s="59" t="s">
         <v>62</v>
@@ -14728,7 +14745,7 @@
         <v>274.53832919643253</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
       <c r="B66" s="59" t="s">
         <v>62</v>
@@ -14798,7 +14815,7 @@
         <v>74.671918177853058</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
       <c r="B67" s="59" t="s">
         <v>62</v>
@@ -14868,7 +14885,7 @@
         <v>52.786854223608252</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="12.95" customHeight="1">
+    <row r="68" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="59" t="s">
         <v>62</v>
       </c>
@@ -14937,7 +14954,7 @@
         <v>682.23047857511699</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="12.95" customHeight="1">
+    <row r="69" spans="1:20" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="59" t="s">
         <v>62</v>
       </c>
@@ -15006,7 +15023,7 @@
         <v>95.13176685151258</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C70" s="2" t="s">
         <v>1</v>
       </c>
@@ -15065,7 +15082,7 @@
         <v>1522.0219336146308</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C71" s="7" t="s">
         <v>0</v>
       </c>
@@ -15124,7 +15141,7 @@
         <v>5480.3501702541162</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C72" s="7"/>
       <c r="D72" s="19"/>
       <c r="E72" s="18"/>
@@ -15133,7 +15150,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="16"/>
     </row>
-    <row r="73" spans="1:20" ht="15">
+    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="C73" s="13"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
@@ -15141,7 +15158,7 @@
       <c r="H73" s="15"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
@@ -15149,18 +15166,18 @@
       <c r="H74" s="10"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H75" s="10"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H76" s="10"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="1:20" ht="15">
+    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
       <c r="C78" s="13"/>
@@ -15170,7 +15187,7 @@
       <c r="G78" s="11"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -15180,7 +15197,7 @@
       <c r="G79" s="8"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="7"/>
@@ -15190,7 +15207,7 @@
       <c r="G80" s="6"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="7"/>
@@ -15200,7 +15217,7 @@
       <c r="G81" s="6"/>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="7"/>
@@ -15210,7 +15227,7 @@
       <c r="G82" s="6"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="7"/>
@@ -15220,7 +15237,7 @@
       <c r="G83" s="6"/>
       <c r="I83" s="4"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="7"/>
@@ -15230,7 +15247,7 @@
       <c r="G84" s="6"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="7"/>
@@ -15240,7 +15257,7 @@
       <c r="G85" s="6"/>
       <c r="I85" s="4"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="7"/>
@@ -15250,7 +15267,7 @@
       <c r="G86" s="6"/>
       <c r="I86" s="4"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="7"/>
@@ -15260,7 +15277,7 @@
       <c r="G87" s="6"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="7"/>
@@ -15270,7 +15287,7 @@
       <c r="G88" s="6"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="7"/>
@@ -15280,7 +15297,7 @@
       <c r="G89" s="6"/>
       <c r="I89" s="4"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="7"/>
@@ -15290,7 +15307,7 @@
       <c r="G90" s="6"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="7"/>
@@ -15300,7 +15317,7 @@
       <c r="G91" s="6"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="7"/>
@@ -15310,7 +15327,7 @@
       <c r="G92" s="6"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="7"/>
@@ -15320,7 +15337,7 @@
       <c r="G93" s="6"/>
       <c r="I93" s="4"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="7"/>
@@ -15330,7 +15347,7 @@
       <c r="G94" s="6"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="7"/>
@@ -15340,7 +15357,7 @@
       <c r="G95" s="6"/>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="7"/>
@@ -15350,7 +15367,7 @@
       <c r="G96" s="6"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="7"/>
@@ -15360,7 +15377,7 @@
       <c r="G97" s="6"/>
       <c r="I97" s="4"/>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="7"/>
@@ -15370,7 +15387,7 @@
       <c r="G98" s="6"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="7"/>
@@ -15380,7 +15397,7 @@
       <c r="G99" s="6"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="7"/>
@@ -15390,7 +15407,7 @@
       <c r="G100" s="6"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="7"/>
@@ -15399,7 +15416,7 @@
       <c r="F101" s="6"/>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="7"/>
@@ -15408,7 +15425,7 @@
       <c r="F102" s="6"/>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="7"/>
@@ -15417,7 +15434,7 @@
       <c r="F103" s="6"/>
       <c r="I103" s="4"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="7"/>
@@ -15426,7 +15443,7 @@
       <c r="F104" s="6"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="7"/>
@@ -15435,7 +15452,7 @@
       <c r="F105" s="6"/>
       <c r="I105" s="4"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="5"/>
       <c r="B106" s="5"/>
       <c r="C106" s="7"/>
@@ -15444,7 +15461,7 @@
       <c r="F106" s="6"/>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="7"/>
@@ -15453,7 +15470,7 @@
       <c r="F107" s="6"/>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
       <c r="C108" s="7"/>
@@ -15462,7 +15479,7 @@
       <c r="F108" s="6"/>
       <c r="I108" s="4"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="7"/>
@@ -15471,7 +15488,7 @@
       <c r="F109" s="6"/>
       <c r="I109" s="4"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
       <c r="C110" s="7"/>
@@ -15480,7 +15497,7 @@
       <c r="F110" s="6"/>
       <c r="I110" s="4"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="7"/>
@@ -15489,37 +15506,37 @@
       <c r="F111" s="6"/>
       <c r="I111" s="4"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
       <c r="D112" s="2"/>
       <c r="I112" s="4"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="2"/>
@@ -15612,7 +15629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
@@ -15622,7 +15639,7 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="7" width="14.85546875" customWidth="1"/>
@@ -15705,7 +15722,7 @@
     <col min="100" max="100" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>64</v>
       </c>
@@ -15734,7 +15751,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>50</v>
       </c>
@@ -15757,7 +15774,7 @@
         <v>179.9794444129509</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>53</v>
       </c>
@@ -15801,7 +15818,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
         <v>12</v>
       </c>
@@ -15845,7 +15862,7 @@
         <v>143.80902935273241</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>46</v>
       </c>
@@ -15889,7 +15906,7 @@
         <v>559.59112663145822</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
         <v>62</v>
       </c>
@@ -15933,7 +15950,7 @@
         <v>1876.3700805076637</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
         <v>63</v>
       </c>
@@ -15977,7 +15994,7 @@
         <v>60.277623624157478</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J8" s="64" t="s">
         <v>62</v>
       </c>
@@ -16000,7 +16017,7 @@
         <v>2879.8200120001902</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J9" s="64" t="s">
         <v>63</v>
       </c>
@@ -16030,19 +16047,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -16065,7 +16082,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -16088,7 +16105,7 @@
         <v>179.9794444129509</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -16111,7 +16128,7 @@
         <v>3456.2999892578664</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -16134,7 +16151,7 @@
         <v>1917.573917246491</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -16157,7 +16174,7 @@
         <v>284.51515620752696</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -16180,7 +16197,7 @@
         <v>3782.845643387971</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="61" t="s">
         <v>63</v>
       </c>
@@ -16215,17 +16232,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F7" workbookViewId="0">
       <selection activeCell="J4" sqref="J4:O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -16265,7 +16282,7 @@
     <col min="52" max="57" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>64</v>
       </c>
@@ -16294,7 +16311,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>50</v>
       </c>
@@ -16317,7 +16334,7 @@
         <v>137.77026292010845</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>53</v>
       </c>
@@ -16361,7 +16378,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
         <v>12</v>
       </c>
@@ -16405,7 +16422,7 @@
         <v>104.84279448741343</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>46</v>
       </c>
@@ -16449,7 +16466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
         <v>62</v>
       </c>
@@ -16493,7 +16510,7 @@
         <v>74.671918177853058</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
         <v>63</v>
       </c>
@@ -16543,28 +16560,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4:AM8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="18.75">
+    <row r="1" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="18.75">
+    <row r="2" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="72" t="s">
         <v>81</v>
       </c>
@@ -16585,7 +16602,7 @@
       </c>
       <c r="AH2" s="61"/>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
         <v>64</v>
       </c>
@@ -16693,7 +16710,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>50</v>
       </c>
@@ -16801,7 +16818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
         <v>53</v>
       </c>
@@ -16909,7 +16926,7 @@
         <v>61.760245373879883</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
         <v>12</v>
       </c>
@@ -17017,7 +17034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>46</v>
       </c>
@@ -17125,7 +17142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
         <v>62</v>
       </c>
@@ -17233,7 +17250,7 @@
         <v>158.15512270069277</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="75" t="s">
         <v>63</v>
       </c>
@@ -17371,7 +17388,7 @@
         <v>219.91536807457265</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="87" customFormat="1">
+    <row r="10" spans="1:39" s="87" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82" t="s">
         <v>86</v>
       </c>
@@ -17429,7 +17446,7 @@
       <c r="AL10" s="86"/>
       <c r="AM10" s="86"/>
     </row>
-    <row r="11" spans="1:39" s="87" customFormat="1">
+    <row r="11" spans="1:39" s="87" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="82"/>
       <c r="B11" s="83"/>
       <c r="C11" s="83"/>
@@ -17467,12 +17484,12 @@
       <c r="AL11" s="86"/>
       <c r="AM11" s="86"/>
     </row>
-    <row r="12" spans="1:39" ht="18.75">
+    <row r="12" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B13" s="78">
         <v>2013</v>
       </c>
@@ -17588,7 +17605,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>50</v>
       </c>
@@ -17744,7 +17761,7 @@
         <v>179.9794444129509</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
         <v>53</v>
       </c>
@@ -17900,7 +17917,7 @@
         <v>3456.2999892578664</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>12</v>
       </c>
@@ -18056,7 +18073,7 @@
         <v>1917.573917246491</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
         <v>46</v>
       </c>
@@ -18212,7 +18229,7 @@
         <v>284.51515620752696</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>62</v>
       </c>
@@ -18368,7 +18385,7 @@
         <v>3782.845643387971</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>78</v>
       </c>
@@ -18526,12 +18543,12 @@
       </c>
       <c r="AN19" s="69"/>
     </row>
-    <row r="21" spans="1:40" ht="18.75">
+    <row r="21" spans="1:40" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B22" s="78">
         <v>2013</v>
       </c>
@@ -18647,7 +18664,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
         <v>50</v>
       </c>
@@ -18803,7 +18820,7 @@
         <v>143.80902935273241</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="74" t="s">
         <v>53</v>
       </c>
@@ -18959,7 +18976,7 @@
         <v>559.59112663145822</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="74" t="s">
         <v>12</v>
       </c>
@@ -19115,7 +19132,7 @@
         <v>1876.3700805076637</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="74" t="s">
         <v>46</v>
       </c>
@@ -19271,7 +19288,7 @@
         <v>60.277623624157478</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="74" t="s">
         <v>62</v>
       </c>
@@ -19427,7 +19444,7 @@
         <v>2879.8200120001902</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" s="74" t="s">
         <v>78</v>
       </c>
@@ -19584,12 +19601,12 @@
         <v>5519.8678721162014</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="18.75">
+    <row r="30" spans="1:40" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="72" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B31" s="78">
         <v>2013</v>
       </c>
@@ -19705,7 +19722,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32" s="74" t="s">
         <v>50</v>
       </c>
@@ -19861,7 +19878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="74" t="s">
         <v>53</v>
       </c>
@@ -20017,7 +20034,7 @@
         <v>1116.5399459675916</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
         <v>12</v>
       </c>
@@ -20173,7 +20190,7 @@
         <v>25.025268913351944</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="74" t="s">
         <v>46</v>
       </c>
@@ -20329,7 +20346,7 @@
         <v>31.26125647993058</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="74" t="s">
         <v>62</v>
       </c>
@@ -20485,7 +20502,7 @@
         <v>68.360166038638383</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="74" t="s">
         <v>78</v>
       </c>
@@ -20642,12 +20659,12 @@
         <v>1241.1866373995126</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="18.75">
+    <row r="39" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="72" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B40" s="78">
         <v>2013</v>
       </c>
@@ -20763,7 +20780,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="74" t="s">
         <v>50</v>
       </c>
@@ -20919,7 +20936,7 @@
         <v>36.170415060218481</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
         <v>53</v>
       </c>
@@ -21075,7 +21092,7 @@
         <v>1718.4086712849364</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="74" t="s">
         <v>12</v>
       </c>
@@ -21231,7 +21248,7 @@
         <v>16.178567825475181</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
         <v>46</v>
       </c>
@@ -21387,7 +21404,7 @@
         <v>192.97627610343889</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="74" t="s">
         <v>62</v>
       </c>
@@ -21543,7 +21560,7 @@
         <v>676.51034264845043</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
         <v>78</v>
       </c>
@@ -21700,12 +21717,12 @@
         <v>2640.2442729225195</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="18.75">
+    <row r="48" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="72" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:39">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B49" s="78">
         <v>2013</v>
       </c>
@@ -21821,7 +21838,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="50" spans="1:39">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
         <v>50</v>
       </c>
@@ -21977,7 +21994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:39">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="s">
         <v>53</v>
       </c>
@@ -22133,7 +22150,7 @@
         <v>61.760245373879883</v>
       </c>
     </row>
-    <row r="52" spans="1:39">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" s="74" t="s">
         <v>12</v>
       </c>
@@ -22289,7 +22306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A53" s="74" t="s">
         <v>46</v>
       </c>
@@ -22445,7 +22462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:39">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A54" s="74" t="s">
         <v>62</v>
       </c>
@@ -22601,7 +22618,7 @@
         <v>158.15512270069277</v>
       </c>
     </row>
-    <row r="55" spans="1:39">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A55" s="74" t="s">
         <v>78</v>
       </c>
@@ -22764,28 +22781,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4:AM8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="18.75">
+    <row r="1" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="18.75">
+    <row r="2" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="72" t="s">
         <v>81</v>
       </c>
@@ -22806,8 +22823,8 @@
       </c>
       <c r="AH2" s="61"/>
     </row>
-    <row r="3" spans="1:39">
-      <c r="A3" s="73" t="s">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="100" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="61">
@@ -22829,7 +22846,7 @@
         <v>2050</v>
       </c>
       <c r="H3" s="70"/>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="100" t="s">
         <v>64</v>
       </c>
       <c r="J3" s="61">
@@ -22850,7 +22867,7 @@
       <c r="O3" s="61">
         <v>2050</v>
       </c>
-      <c r="Q3" s="73" t="s">
+      <c r="Q3" s="100" t="s">
         <v>64</v>
       </c>
       <c r="R3" s="61">
@@ -22871,7 +22888,7 @@
       <c r="W3" s="61">
         <v>2050</v>
       </c>
-      <c r="Y3" s="73" t="s">
+      <c r="Y3" s="100" t="s">
         <v>64</v>
       </c>
       <c r="Z3" s="61">
@@ -22892,7 +22909,7 @@
       <c r="AE3" s="61">
         <v>2050</v>
       </c>
-      <c r="AG3" s="73" t="s">
+      <c r="AG3" s="100" t="s">
         <v>64</v>
       </c>
       <c r="AH3" s="61">
@@ -22914,8 +22931,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
-      <c r="A4" s="74" t="s">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="99" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="65">
@@ -22937,7 +22954,7 @@
         <v>137.77026292010845</v>
       </c>
       <c r="H4" s="70"/>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="99" t="s">
         <v>50</v>
       </c>
       <c r="J4" s="80">
@@ -22958,7 +22975,7 @@
       <c r="O4" s="80">
         <v>101.59984785988996</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="Q4" s="99" t="s">
         <v>50</v>
       </c>
       <c r="R4" s="68">
@@ -22979,7 +22996,7 @@
       <c r="W4" s="68">
         <v>0</v>
       </c>
-      <c r="Y4" s="74" t="s">
+      <c r="Y4" s="99" t="s">
         <v>50</v>
       </c>
       <c r="Z4" s="68">
@@ -23000,7 +23017,7 @@
       <c r="AE4" s="68">
         <v>36.170415060218481</v>
       </c>
-      <c r="AG4" s="74" t="s">
+      <c r="AG4" s="99" t="s">
         <v>50</v>
       </c>
       <c r="AH4" s="68">
@@ -23022,8 +23039,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
-      <c r="A5" s="74" t="s">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="99" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="65">
@@ -23045,7 +23062,7 @@
         <v>2208.2131574502509</v>
       </c>
       <c r="H5" s="70"/>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="99" t="s">
         <v>53</v>
       </c>
       <c r="J5" s="80">
@@ -23066,7 +23083,7 @@
       <c r="O5" s="80">
         <v>402.13701746530143</v>
       </c>
-      <c r="Q5" s="74" t="s">
+      <c r="Q5" s="99" t="s">
         <v>53</v>
       </c>
       <c r="R5" s="68">
@@ -23087,7 +23104,7 @@
       <c r="W5" s="68">
         <v>864.71938608943913</v>
       </c>
-      <c r="Y5" s="74" t="s">
+      <c r="Y5" s="99" t="s">
         <v>53</v>
       </c>
       <c r="Z5" s="68">
@@ -23108,7 +23125,7 @@
       <c r="AE5" s="68">
         <v>836.51395940809687</v>
       </c>
-      <c r="AG5" s="74" t="s">
+      <c r="AG5" s="99" t="s">
         <v>53</v>
       </c>
       <c r="AH5" s="68">
@@ -23130,8 +23147,8 @@
         <v>104.84279448741343</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
-      <c r="A6" s="74" t="s">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="65">
@@ -23153,7 +23170,7 @@
         <v>1495.8025667488926</v>
       </c>
       <c r="H6" s="70"/>
-      <c r="I6" s="74" t="s">
+      <c r="I6" s="99" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="80">
@@ -23174,7 +23191,7 @@
       <c r="O6" s="80">
         <v>1346.8790390140794</v>
       </c>
-      <c r="Q6" s="74" t="s">
+      <c r="Q6" s="99" t="s">
         <v>12</v>
       </c>
       <c r="R6" s="68">
@@ -23195,7 +23212,7 @@
       <c r="W6" s="68">
         <v>54.99100619764036</v>
       </c>
-      <c r="Y6" s="74" t="s">
+      <c r="Y6" s="99" t="s">
         <v>12</v>
       </c>
       <c r="Z6" s="68">
@@ -23216,7 +23233,7 @@
       <c r="AE6" s="68">
         <v>93.93252153717259</v>
       </c>
-      <c r="AG6" s="74" t="s">
+      <c r="AG6" s="99" t="s">
         <v>12</v>
       </c>
       <c r="AH6" s="68">
@@ -23238,8 +23255,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
-      <c r="A7" s="74" t="s">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="65">
@@ -23261,7 +23278,7 @@
         <v>116.54224952023492</v>
       </c>
       <c r="H7" s="70"/>
-      <c r="I7" s="74" t="s">
+      <c r="I7" s="99" t="s">
         <v>46</v>
       </c>
       <c r="J7" s="80">
@@ -23282,7 +23299,7 @@
       <c r="O7" s="80">
         <v>40.332096399023833</v>
       </c>
-      <c r="Q7" s="74" t="s">
+      <c r="Q7" s="99" t="s">
         <v>46</v>
       </c>
       <c r="R7" s="68">
@@ -23303,7 +23320,7 @@
       <c r="W7" s="68">
         <v>20.917088617477368</v>
       </c>
-      <c r="Y7" s="74" t="s">
+      <c r="Y7" s="99" t="s">
         <v>46</v>
       </c>
       <c r="Z7" s="68">
@@ -23324,7 +23341,7 @@
       <c r="AE7" s="68">
         <v>55.293064503733717</v>
       </c>
-      <c r="AG7" s="74" t="s">
+      <c r="AG7" s="99" t="s">
         <v>46</v>
       </c>
       <c r="AH7" s="68">
@@ -23346,8 +23363,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
-      <c r="A8" s="74" t="s">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="99" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="65">
@@ -23369,7 +23386,7 @@
         <v>1522.0219336146306</v>
       </c>
       <c r="H8" s="71"/>
-      <c r="I8" s="74" t="s">
+      <c r="I8" s="99" t="s">
         <v>62</v>
       </c>
       <c r="J8" s="80">
@@ -23390,7 +23407,7 @@
       <c r="O8" s="80">
         <v>958.44313514135695</v>
       </c>
-      <c r="Q8" s="74" t="s">
+      <c r="Q8" s="99" t="s">
         <v>62</v>
       </c>
       <c r="R8" s="68">
@@ -23411,7 +23428,7 @@
       <c r="W8" s="68">
         <v>66.449930023867523</v>
       </c>
-      <c r="Y8" s="74" t="s">
+      <c r="Y8" s="99" t="s">
         <v>62</v>
       </c>
       <c r="Z8" s="68">
@@ -23432,7 +23449,7 @@
       <c r="AE8" s="68">
         <v>422.45695027155335</v>
       </c>
-      <c r="AG8" s="74" t="s">
+      <c r="AG8" s="99" t="s">
         <v>62</v>
       </c>
       <c r="AH8" s="68">
@@ -23454,8 +23471,8 @@
         <v>74.671918177853058</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
-      <c r="A9" s="75" t="s">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="101" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="66">
@@ -23483,7 +23500,7 @@
         <v>5480.350170254118</v>
       </c>
       <c r="H9" s="71"/>
-      <c r="I9" s="75" t="s">
+      <c r="I9" s="101" t="s">
         <v>63</v>
       </c>
       <c r="J9" s="66">
@@ -23510,7 +23527,7 @@
         <f t="shared" si="1"/>
         <v>2849.3911358796518</v>
       </c>
-      <c r="Q9" s="75" t="s">
+      <c r="Q9" s="101" t="s">
         <v>63</v>
       </c>
       <c r="R9" s="66">
@@ -23537,7 +23554,7 @@
         <f t="shared" si="2"/>
         <v>1007.0774109284243</v>
       </c>
-      <c r="Y9" s="75" t="s">
+      <c r="Y9" s="101" t="s">
         <v>63</v>
       </c>
       <c r="Z9" s="66">
@@ -23564,7 +23581,7 @@
         <f t="shared" si="3"/>
         <v>1444.366910780775</v>
       </c>
-      <c r="AG9" s="75" t="s">
+      <c r="AG9" s="101" t="s">
         <v>63</v>
       </c>
       <c r="AH9" s="66">
@@ -23592,7 +23609,7 @@
         <v>179.51471266526647</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="87" customFormat="1">
+    <row r="10" spans="1:39" s="87" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82" t="s">
         <v>86</v>
       </c>
@@ -23650,7 +23667,7 @@
       <c r="AL10" s="86"/>
       <c r="AM10" s="86"/>
     </row>
-    <row r="11" spans="1:39" s="87" customFormat="1">
+    <row r="11" spans="1:39" s="87" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="82"/>
       <c r="B11" s="83"/>
       <c r="C11" s="83"/>
@@ -23688,12 +23705,12 @@
       <c r="AL11" s="86"/>
       <c r="AM11" s="86"/>
     </row>
-    <row r="12" spans="1:39" ht="18.75">
+    <row r="12" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B13" s="78">
         <v>2013</v>
       </c>
@@ -23809,8 +23826,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
-      <c r="A14" s="74" t="s">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="99" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="77">
@@ -23965,8 +23982,8 @@
         <v>137.77026292010845</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
-      <c r="A15" s="74" t="s">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="99" t="s">
         <v>53</v>
       </c>
       <c r="B15" s="77">
@@ -24121,8 +24138,8 @@
         <v>2208.2131574502509</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
-      <c r="A16" s="74" t="s">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="77">
@@ -24277,8 +24294,8 @@
         <v>1495.8025667488926</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
-      <c r="A17" s="74" t="s">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="77">
@@ -24433,8 +24450,8 @@
         <v>116.54224952023492</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
-      <c r="A18" s="74" t="s">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A18" s="99" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="77">
@@ -24589,8 +24606,8 @@
         <v>1522.0219336146306</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
-      <c r="A19" s="74" t="s">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A19" s="99" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="79">
@@ -24747,12 +24764,12 @@
       </c>
       <c r="AN19" s="69"/>
     </row>
-    <row r="21" spans="1:40" ht="18.75">
+    <row r="21" spans="1:40" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B22" s="78">
         <v>2013</v>
       </c>
@@ -24868,8 +24885,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
-      <c r="A23" s="74" t="s">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A23" s="99" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="77">
@@ -25024,8 +25041,8 @@
         <v>101.59984785988996</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
-      <c r="A24" s="74" t="s">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A24" s="99" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="77">
@@ -25180,8 +25197,8 @@
         <v>402.13701746530143</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
-      <c r="A25" s="74" t="s">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="77">
@@ -25336,8 +25353,8 @@
         <v>1346.8790390140794</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
-      <c r="A26" s="74" t="s">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="77">
@@ -25492,8 +25509,8 @@
         <v>40.332096399023833</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
-      <c r="A27" s="74" t="s">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27" s="99" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="77">
@@ -25648,8 +25665,8 @@
         <v>958.44313514135695</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
-      <c r="A28" s="74" t="s">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A28" s="99" t="s">
         <v>78</v>
       </c>
       <c r="B28" s="79">
@@ -25805,12 +25822,12 @@
         <v>2849.3911358796518</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="18.75">
+    <row r="30" spans="1:40" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="72" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B31" s="78">
         <v>2013</v>
       </c>
@@ -25926,8 +25943,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
-      <c r="A32" s="74" t="s">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A32" s="99" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="77">
@@ -26082,8 +26099,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
-      <c r="A33" s="74" t="s">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" s="99" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="77">
@@ -26238,8 +26255,8 @@
         <v>864.71938608943913</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
-      <c r="A34" s="74" t="s">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="77">
@@ -26394,8 +26411,8 @@
         <v>54.99100619764036</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
-      <c r="A35" s="74" t="s">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="77">
@@ -26550,8 +26567,8 @@
         <v>20.917088617477368</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
-      <c r="A36" s="74" t="s">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" s="99" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="77">
@@ -26706,8 +26723,8 @@
         <v>66.449930023867523</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
-      <c r="A37" s="74" t="s">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" s="99" t="s">
         <v>78</v>
       </c>
       <c r="B37" s="79">
@@ -26863,12 +26880,12 @@
         <v>1007.0774109284243</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="18.75">
+    <row r="39" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="72" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B40" s="78">
         <v>2013</v>
       </c>
@@ -26984,8 +27001,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
-      <c r="A41" s="74" t="s">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="99" t="s">
         <v>50</v>
       </c>
       <c r="B41" s="77">
@@ -27140,8 +27157,8 @@
         <v>36.170415060218481</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
-      <c r="A42" s="74" t="s">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="99" t="s">
         <v>53</v>
       </c>
       <c r="B42" s="77">
@@ -27296,8 +27313,8 @@
         <v>836.51395940809687</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
-      <c r="A43" s="74" t="s">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="77">
@@ -27452,8 +27469,8 @@
         <v>93.93252153717259</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
-      <c r="A44" s="74" t="s">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="77">
@@ -27608,8 +27625,8 @@
         <v>55.293064503733717</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
-      <c r="A45" s="74" t="s">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="99" t="s">
         <v>62</v>
       </c>
       <c r="B45" s="77">
@@ -27764,8 +27781,8 @@
         <v>422.45695027155335</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
-      <c r="A46" s="74" t="s">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" s="99" t="s">
         <v>78</v>
       </c>
       <c r="B46" s="79">
@@ -27921,12 +27938,12 @@
         <v>1444.366910780775</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="18.75">
+    <row r="48" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="72" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:39">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B49" s="78">
         <v>2013</v>
       </c>
@@ -28042,8 +28059,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="50" spans="1:39">
-      <c r="A50" s="74" t="s">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A50" s="99" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="77">
@@ -28198,8 +28215,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:39">
-      <c r="A51" s="74" t="s">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A51" s="99" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="77">
@@ -28354,8 +28371,8 @@
         <v>104.84279448741343</v>
       </c>
     </row>
-    <row r="52" spans="1:39">
-      <c r="A52" s="74" t="s">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A52" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="77">
@@ -28510,8 +28527,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
-      <c r="A53" s="74" t="s">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A53" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B53" s="77">
@@ -28666,8 +28683,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:39">
-      <c r="A54" s="74" t="s">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A54" s="99" t="s">
         <v>62</v>
       </c>
       <c r="B54" s="77">
@@ -28822,8 +28839,8 @@
         <v>74.671918177853058</v>
       </c>
     </row>
-    <row r="55" spans="1:39">
-      <c r="A55" s="74" t="s">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A55" s="99" t="s">
         <v>78</v>
       </c>
       <c r="B55" s="79">
@@ -28985,21 +29002,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="45" customWidth="1"/>
     <col min="5" max="5" width="111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:5">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>26</v>
       </c>
@@ -29011,7 +29028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="16.5" thickBot="1">
+    <row r="3" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24">
         <v>1</v>
       </c>
@@ -29025,7 +29042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="16.5" thickBot="1">
+    <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24">
         <v>2</v>
       </c>
@@ -29037,7 +29054,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="16.5" thickBot="1">
+    <row r="5" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24">
         <v>3</v>
       </c>
@@ -29049,7 +29066,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="16.5" thickBot="1">
+    <row r="6" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24">
         <v>4</v>
       </c>
@@ -29061,7 +29078,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="16.5" thickBot="1">
+    <row r="7" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24">
         <v>5</v>
       </c>
@@ -29073,7 +29090,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="16.5" thickBot="1">
+    <row r="8" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24">
         <v>6</v>
       </c>
@@ -29085,7 +29102,7 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="16.5" thickBot="1">
+    <row r="9" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24">
         <v>7</v>
       </c>
@@ -29097,7 +29114,7 @@
         <v>3311</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="16.5" thickBot="1">
+    <row r="10" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="24">
         <v>8</v>
       </c>
@@ -29109,7 +29126,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="16.5" thickBot="1">
+    <row r="11" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="24">
         <v>9</v>
       </c>
@@ -29121,7 +29138,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="16.5" thickBot="1">
+    <row r="12" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="24">
         <v>10</v>
       </c>
@@ -29133,7 +29150,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="16.5" thickBot="1">
+    <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24">
         <v>11</v>
       </c>
@@ -29145,7 +29162,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="16.5" thickBot="1">
+    <row r="14" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24">
         <v>12</v>
       </c>
@@ -29159,7 +29176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="16.5" thickBot="1">
+    <row r="15" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="24">
         <v>13</v>
       </c>
@@ -29171,7 +29188,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="16.5" thickBot="1">
+    <row r="16" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="24">
         <v>14</v>
       </c>
@@ -29183,7 +29200,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="16.5" thickBot="1">
+    <row r="17" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="24">
         <v>15</v>
       </c>
@@ -29195,7 +29212,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="16.5" thickBot="1">
+    <row r="18" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="24">
         <v>16</v>
       </c>
@@ -29207,7 +29224,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="16.5" thickBot="1">
+    <row r="19" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="24">
         <v>17</v>
       </c>
@@ -29219,7 +29236,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="63.75" customHeight="1" thickBot="1">
+    <row r="20" spans="2:5" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="31">
         <v>18</v>
       </c>
@@ -29233,7 +29250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="16.5" thickBot="1">
+    <row r="21" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="34">
         <v>19</v>
       </c>
@@ -29245,7 +29262,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="16.5" thickBot="1">
+    <row r="22" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="31">
         <v>20</v>
       </c>
@@ -29259,7 +29276,7 @@
         <v>3241</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="16.5" thickBot="1">
+    <row r="23" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="34">
         <v>21</v>
       </c>
@@ -29271,7 +29288,7 @@
         <v>2222</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="15.75">
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="31">
         <v>22</v>
       </c>
@@ -29295,19 +29312,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Calibration energy in the baseline using solver and energy productivity as control variable
</commit_message>
<xml_diff>
--- a/data/database/DATA_Enerdata_input ThreeMe.xlsx
+++ b/data/database/DATA_Enerdata_input ThreeMe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Energy final consumption-Mtoe" sheetId="1" r:id="rId1"/>
@@ -1060,6 +1060,13 @@
     </xf>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1093,13 +1100,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Milliers 3" xfId="3"/>
@@ -1110,13 +1110,7 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -1269,7 +1263,13 @@
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -4423,469 +4423,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I3:O7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item x="4"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="23">
-        <item x="0"/>
-        <item x="10"/>
-        <item x="21"/>
-        <item x="8"/>
-        <item x="19"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="18"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="11"/>
-        <item x="20"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="8">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item h="1" x="5"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
-      <items count="5">
-        <item sd="0" x="1"/>
-        <item n="Oil&amp;Coal" h="1" sd="0" x="3"/>
-        <item n="Elec&amp;Solar" h="1" sd="0" x="4"/>
-        <item h="1" sd="0" x="0"/>
-        <item h="1" x="2"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="9" hier="-1"/>
-  </pageFields>
-  <dataFields count="6">
-    <dataField name="Somme de 2014" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2020" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2025" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2030" fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2040" fld="7" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="32">
-    <format dxfId="31">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="26">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="19"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="21">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="20">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="18">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="17">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="15">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="14">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="16"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="11">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="20"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="10">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="15"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="17"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="5">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="18"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="21"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="2">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
@@ -5013,6 +4550,835 @@
     <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="51">
+    <format dxfId="50">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="49">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="48">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="47">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="46">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="44">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="43">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="41">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="40">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="37">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="19"/>
+          </reference>
+          <reference field="2" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="14"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="16"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="20"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="20"/>
+          </reference>
+          <reference field="2" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="15"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="17"/>
+          </reference>
+          <reference field="2" count="3">
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="18"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="21"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="21"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I3:O7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item x="4"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="23">
+        <item x="0"/>
+        <item x="10"/>
+        <item x="21"/>
+        <item x="8"/>
+        <item x="19"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item x="18"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="17"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="11"/>
+        <item x="20"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item h="1" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item sd="0" x="1"/>
+        <item n="Oil&amp;Coal" h="1" sd="0" x="3"/>
+        <item n="Elec&amp;Solar" h="1" sd="0" x="4"/>
+        <item h="1" sd="0" x="0"/>
+        <item h="1" x="2"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="9" hier="-1"/>
+  </pageFields>
+  <dataFields count="6">
+    <dataField name="Somme de 2014" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2020" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2025" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2030" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2040" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="32">
     <format dxfId="82">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
@@ -5036,25 +5402,21 @@
     </format>
     <format dxfId="80">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="79">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
             <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
@@ -5066,54 +5428,12 @@
             <x v="1"/>
           </reference>
           <reference field="1" count="1">
-            <x v="4"/>
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="77">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="76">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="75">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="74">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5125,22 +5445,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="12"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="72">
+    <format dxfId="76">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -5149,7 +5454,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="75">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5161,23 +5466,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="69">
+    <format dxfId="74">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5189,31 +5478,83 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="73">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="70">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="68">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
+        <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="5"/>
+            <x v="2"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="19"/>
-          </reference>
-          <reference field="2" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
+          <reference field="1" count="1">
+            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
             <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="11"/>
           </reference>
         </references>
       </pivotArea>
@@ -5225,23 +5566,19 @@
             <x v="2"/>
           </reference>
           <reference field="1" count="1">
-            <x v="3"/>
+            <x v="13"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
+        <references count="2">
           <reference field="0" count="1" selected="0">
             <x v="2"/>
           </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="3"/>
+          <reference field="1" count="1">
+            <x v="14"/>
           </reference>
         </references>
       </pivotArea>
@@ -5253,244 +5590,12 @@
             <x v="2"/>
           </reference>
           <reference field="1" count="1">
-            <x v="5"/>
+            <x v="16"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="63">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="62">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="61">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="60">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="59">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="58">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="57">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="56">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="55">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="11"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="54">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="53">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="13"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="52">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="51">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="14"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="50">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="16"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="49">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="16"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="48">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -5499,7 +5604,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5511,27 +5616,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="20"/>
-          </reference>
-          <reference field="2" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
+    <format dxfId="61">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -5540,7 +5625,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5552,22 +5637,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="42">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5579,23 +5649,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="40">
+    <format dxfId="58">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5607,22 +5661,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="15"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
+    <format dxfId="57">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5634,24 +5673,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="17"/>
-          </reference>
-          <reference field="2" count="3">
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5663,23 +5685,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="18"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="34">
+    <format dxfId="55">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5691,23 +5697,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="21"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
+    <format dxfId="54">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    <format dxfId="53">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="52">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="51">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -5762,7 +5762,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5797,7 +5797,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -6006,25 +6006,25 @@
         <v>74</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="90"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
       <c r="M1" s="60"/>
-      <c r="O1" s="88" t="s">
+      <c r="O1" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="90"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="93"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
@@ -10458,25 +10458,25 @@
         <v>74</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="90"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
       <c r="M1" s="60"/>
-      <c r="O1" s="88" t="s">
+      <c r="O1" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="90"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="93"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
@@ -16566,8 +16566,8 @@
   </sheetPr>
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4:AM8"/>
+    <sheetView tabSelected="1" topLeftCell="U22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:AM45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22787,8 +22787,8 @@
   </sheetPr>
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4:AM8"/>
+    <sheetView topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:AI46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22824,7 +22824,7 @@
       <c r="AH2" s="61"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="89" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="61">
@@ -22846,7 +22846,7 @@
         <v>2050</v>
       </c>
       <c r="H3" s="70"/>
-      <c r="I3" s="100" t="s">
+      <c r="I3" s="89" t="s">
         <v>64</v>
       </c>
       <c r="J3" s="61">
@@ -22867,7 +22867,7 @@
       <c r="O3" s="61">
         <v>2050</v>
       </c>
-      <c r="Q3" s="100" t="s">
+      <c r="Q3" s="89" t="s">
         <v>64</v>
       </c>
       <c r="R3" s="61">
@@ -22888,7 +22888,7 @@
       <c r="W3" s="61">
         <v>2050</v>
       </c>
-      <c r="Y3" s="100" t="s">
+      <c r="Y3" s="89" t="s">
         <v>64</v>
       </c>
       <c r="Z3" s="61">
@@ -22909,7 +22909,7 @@
       <c r="AE3" s="61">
         <v>2050</v>
       </c>
-      <c r="AG3" s="100" t="s">
+      <c r="AG3" s="89" t="s">
         <v>64</v>
       </c>
       <c r="AH3" s="61">
@@ -22932,7 +22932,7 @@
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="88" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="65">
@@ -22954,7 +22954,7 @@
         <v>137.77026292010845</v>
       </c>
       <c r="H4" s="70"/>
-      <c r="I4" s="99" t="s">
+      <c r="I4" s="88" t="s">
         <v>50</v>
       </c>
       <c r="J4" s="80">
@@ -22975,7 +22975,7 @@
       <c r="O4" s="80">
         <v>101.59984785988996</v>
       </c>
-      <c r="Q4" s="99" t="s">
+      <c r="Q4" s="88" t="s">
         <v>50</v>
       </c>
       <c r="R4" s="68">
@@ -22996,7 +22996,7 @@
       <c r="W4" s="68">
         <v>0</v>
       </c>
-      <c r="Y4" s="99" t="s">
+      <c r="Y4" s="88" t="s">
         <v>50</v>
       </c>
       <c r="Z4" s="68">
@@ -23017,7 +23017,7 @@
       <c r="AE4" s="68">
         <v>36.170415060218481</v>
       </c>
-      <c r="AG4" s="99" t="s">
+      <c r="AG4" s="88" t="s">
         <v>50</v>
       </c>
       <c r="AH4" s="68">
@@ -23040,7 +23040,7 @@
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="88" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="65">
@@ -23062,7 +23062,7 @@
         <v>2208.2131574502509</v>
       </c>
       <c r="H5" s="70"/>
-      <c r="I5" s="99" t="s">
+      <c r="I5" s="88" t="s">
         <v>53</v>
       </c>
       <c r="J5" s="80">
@@ -23083,7 +23083,7 @@
       <c r="O5" s="80">
         <v>402.13701746530143</v>
       </c>
-      <c r="Q5" s="99" t="s">
+      <c r="Q5" s="88" t="s">
         <v>53</v>
       </c>
       <c r="R5" s="68">
@@ -23104,7 +23104,7 @@
       <c r="W5" s="68">
         <v>864.71938608943913</v>
       </c>
-      <c r="Y5" s="99" t="s">
+      <c r="Y5" s="88" t="s">
         <v>53</v>
       </c>
       <c r="Z5" s="68">
@@ -23125,7 +23125,7 @@
       <c r="AE5" s="68">
         <v>836.51395940809687</v>
       </c>
-      <c r="AG5" s="99" t="s">
+      <c r="AG5" s="88" t="s">
         <v>53</v>
       </c>
       <c r="AH5" s="68">
@@ -23148,7 +23148,7 @@
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="65">
@@ -23170,7 +23170,7 @@
         <v>1495.8025667488926</v>
       </c>
       <c r="H6" s="70"/>
-      <c r="I6" s="99" t="s">
+      <c r="I6" s="88" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="80">
@@ -23191,7 +23191,7 @@
       <c r="O6" s="80">
         <v>1346.8790390140794</v>
       </c>
-      <c r="Q6" s="99" t="s">
+      <c r="Q6" s="88" t="s">
         <v>12</v>
       </c>
       <c r="R6" s="68">
@@ -23212,7 +23212,7 @@
       <c r="W6" s="68">
         <v>54.99100619764036</v>
       </c>
-      <c r="Y6" s="99" t="s">
+      <c r="Y6" s="88" t="s">
         <v>12</v>
       </c>
       <c r="Z6" s="68">
@@ -23233,7 +23233,7 @@
       <c r="AE6" s="68">
         <v>93.93252153717259</v>
       </c>
-      <c r="AG6" s="99" t="s">
+      <c r="AG6" s="88" t="s">
         <v>12</v>
       </c>
       <c r="AH6" s="68">
@@ -23256,7 +23256,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="88" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="65">
@@ -23278,7 +23278,7 @@
         <v>116.54224952023492</v>
       </c>
       <c r="H7" s="70"/>
-      <c r="I7" s="99" t="s">
+      <c r="I7" s="88" t="s">
         <v>46</v>
       </c>
       <c r="J7" s="80">
@@ -23299,7 +23299,7 @@
       <c r="O7" s="80">
         <v>40.332096399023833</v>
       </c>
-      <c r="Q7" s="99" t="s">
+      <c r="Q7" s="88" t="s">
         <v>46</v>
       </c>
       <c r="R7" s="68">
@@ -23320,7 +23320,7 @@
       <c r="W7" s="68">
         <v>20.917088617477368</v>
       </c>
-      <c r="Y7" s="99" t="s">
+      <c r="Y7" s="88" t="s">
         <v>46</v>
       </c>
       <c r="Z7" s="68">
@@ -23341,7 +23341,7 @@
       <c r="AE7" s="68">
         <v>55.293064503733717</v>
       </c>
-      <c r="AG7" s="99" t="s">
+      <c r="AG7" s="88" t="s">
         <v>46</v>
       </c>
       <c r="AH7" s="68">
@@ -23364,7 +23364,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="88" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="65">
@@ -23386,7 +23386,7 @@
         <v>1522.0219336146306</v>
       </c>
       <c r="H8" s="71"/>
-      <c r="I8" s="99" t="s">
+      <c r="I8" s="88" t="s">
         <v>62</v>
       </c>
       <c r="J8" s="80">
@@ -23407,7 +23407,7 @@
       <c r="O8" s="80">
         <v>958.44313514135695</v>
       </c>
-      <c r="Q8" s="99" t="s">
+      <c r="Q8" s="88" t="s">
         <v>62</v>
       </c>
       <c r="R8" s="68">
@@ -23428,7 +23428,7 @@
       <c r="W8" s="68">
         <v>66.449930023867523</v>
       </c>
-      <c r="Y8" s="99" t="s">
+      <c r="Y8" s="88" t="s">
         <v>62</v>
       </c>
       <c r="Z8" s="68">
@@ -23449,7 +23449,7 @@
       <c r="AE8" s="68">
         <v>422.45695027155335</v>
       </c>
-      <c r="AG8" s="99" t="s">
+      <c r="AG8" s="88" t="s">
         <v>62</v>
       </c>
       <c r="AH8" s="68">
@@ -23472,7 +23472,7 @@
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="90" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="66">
@@ -23500,7 +23500,7 @@
         <v>5480.350170254118</v>
       </c>
       <c r="H9" s="71"/>
-      <c r="I9" s="101" t="s">
+      <c r="I9" s="90" t="s">
         <v>63</v>
       </c>
       <c r="J9" s="66">
@@ -23527,7 +23527,7 @@
         <f t="shared" si="1"/>
         <v>2849.3911358796518</v>
       </c>
-      <c r="Q9" s="101" t="s">
+      <c r="Q9" s="90" t="s">
         <v>63</v>
       </c>
       <c r="R9" s="66">
@@ -23554,7 +23554,7 @@
         <f t="shared" si="2"/>
         <v>1007.0774109284243</v>
       </c>
-      <c r="Y9" s="101" t="s">
+      <c r="Y9" s="90" t="s">
         <v>63</v>
       </c>
       <c r="Z9" s="66">
@@ -23581,7 +23581,7 @@
         <f t="shared" si="3"/>
         <v>1444.366910780775</v>
       </c>
-      <c r="AG9" s="101" t="s">
+      <c r="AG9" s="90" t="s">
         <v>63</v>
       </c>
       <c r="AH9" s="66">
@@ -23827,7 +23827,7 @@
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="88" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="77">
@@ -23983,7 +23983,7 @@
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="88" t="s">
         <v>53</v>
       </c>
       <c r="B15" s="77">
@@ -24139,7 +24139,7 @@
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="77">
@@ -24295,7 +24295,7 @@
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="88" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="77">
@@ -24451,7 +24451,7 @@
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="99" t="s">
+      <c r="A18" s="88" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="77">
@@ -24607,7 +24607,7 @@
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="99" t="s">
+      <c r="A19" s="88" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="79">
@@ -24886,7 +24886,7 @@
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="99" t="s">
+      <c r="A23" s="88" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="77">
@@ -25042,7 +25042,7 @@
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="99" t="s">
+      <c r="A24" s="88" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="77">
@@ -25198,7 +25198,7 @@
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="77">
@@ -25354,7 +25354,7 @@
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="99" t="s">
+      <c r="A26" s="88" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="77">
@@ -25510,7 +25510,7 @@
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="99" t="s">
+      <c r="A27" s="88" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="77">
@@ -25666,7 +25666,7 @@
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="99" t="s">
+      <c r="A28" s="88" t="s">
         <v>78</v>
       </c>
       <c r="B28" s="79">
@@ -25944,7 +25944,7 @@
       </c>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="99" t="s">
+      <c r="A32" s="88" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="77">
@@ -26100,7 +26100,7 @@
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A33" s="99" t="s">
+      <c r="A33" s="88" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="77">
@@ -26256,7 +26256,7 @@
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A34" s="99" t="s">
+      <c r="A34" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="77">
@@ -26412,7 +26412,7 @@
       </c>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A35" s="99" t="s">
+      <c r="A35" s="88" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="77">
@@ -26568,7 +26568,7 @@
       </c>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A36" s="99" t="s">
+      <c r="A36" s="88" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="77">
@@ -26724,7 +26724,7 @@
       </c>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="88" t="s">
         <v>78</v>
       </c>
       <c r="B37" s="79">
@@ -27002,7 +27002,7 @@
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A41" s="99" t="s">
+      <c r="A41" s="88" t="s">
         <v>50</v>
       </c>
       <c r="B41" s="77">
@@ -27158,7 +27158,7 @@
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A42" s="99" t="s">
+      <c r="A42" s="88" t="s">
         <v>53</v>
       </c>
       <c r="B42" s="77">
@@ -27314,7 +27314,7 @@
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A43" s="99" t="s">
+      <c r="A43" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="77">
@@ -27470,7 +27470,7 @@
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A44" s="99" t="s">
+      <c r="A44" s="88" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="77">
@@ -27626,7 +27626,7 @@
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A45" s="99" t="s">
+      <c r="A45" s="88" t="s">
         <v>62</v>
       </c>
       <c r="B45" s="77">
@@ -27782,7 +27782,7 @@
       </c>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A46" s="99" t="s">
+      <c r="A46" s="88" t="s">
         <v>78</v>
       </c>
       <c r="B46" s="79">
@@ -28060,7 +28060,7 @@
       </c>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A50" s="99" t="s">
+      <c r="A50" s="88" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="77">
@@ -28216,7 +28216,7 @@
       </c>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A51" s="99" t="s">
+      <c r="A51" s="88" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="77">
@@ -28372,7 +28372,7 @@
       </c>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A52" s="99" t="s">
+      <c r="A52" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="77">
@@ -28528,7 +28528,7 @@
       </c>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A53" s="99" t="s">
+      <c r="A53" s="88" t="s">
         <v>46</v>
       </c>
       <c r="B53" s="77">
@@ -28684,7 +28684,7 @@
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A54" s="99" t="s">
+      <c r="A54" s="88" t="s">
         <v>62</v>
       </c>
       <c r="B54" s="77">
@@ -28840,7 +28840,7 @@
       </c>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A55" s="99" t="s">
+      <c r="A55" s="88" t="s">
         <v>78</v>
       </c>
       <c r="B55" s="79">
@@ -29032,7 +29032,7 @@
       <c r="B3" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="94" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="25" t="s">
@@ -29046,7 +29046,7 @@
       <c r="B4" s="24">
         <v>2</v>
       </c>
-      <c r="C4" s="92"/>
+      <c r="C4" s="95"/>
       <c r="D4" s="27" t="s">
         <v>24</v>
       </c>
@@ -29058,7 +29058,7 @@
       <c r="B5" s="24">
         <v>3</v>
       </c>
-      <c r="C5" s="92"/>
+      <c r="C5" s="95"/>
       <c r="D5" s="27" t="s">
         <v>23</v>
       </c>
@@ -29070,7 +29070,7 @@
       <c r="B6" s="24">
         <v>4</v>
       </c>
-      <c r="C6" s="92"/>
+      <c r="C6" s="95"/>
       <c r="D6" s="27" t="s">
         <v>22</v>
       </c>
@@ -29082,7 +29082,7 @@
       <c r="B7" s="24">
         <v>5</v>
       </c>
-      <c r="C7" s="92"/>
+      <c r="C7" s="95"/>
       <c r="D7" s="27" t="s">
         <v>21</v>
       </c>
@@ -29094,7 +29094,7 @@
       <c r="B8" s="24">
         <v>6</v>
       </c>
-      <c r="C8" s="92"/>
+      <c r="C8" s="95"/>
       <c r="D8" s="27" t="s">
         <v>20</v>
       </c>
@@ -29106,7 +29106,7 @@
       <c r="B9" s="24">
         <v>7</v>
       </c>
-      <c r="C9" s="92"/>
+      <c r="C9" s="95"/>
       <c r="D9" s="27" t="s">
         <v>19</v>
       </c>
@@ -29118,7 +29118,7 @@
       <c r="B10" s="24">
         <v>8</v>
       </c>
-      <c r="C10" s="92"/>
+      <c r="C10" s="95"/>
       <c r="D10" s="27" t="s">
         <v>18</v>
       </c>
@@ -29130,7 +29130,7 @@
       <c r="B11" s="24">
         <v>9</v>
       </c>
-      <c r="C11" s="92"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="27" t="s">
         <v>17</v>
       </c>
@@ -29142,7 +29142,7 @@
       <c r="B12" s="24">
         <v>10</v>
       </c>
-      <c r="C12" s="92"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="27" t="s">
         <v>16</v>
       </c>
@@ -29154,7 +29154,7 @@
       <c r="B13" s="24">
         <v>11</v>
       </c>
-      <c r="C13" s="93"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="27" t="s">
         <v>15</v>
       </c>
@@ -29166,7 +29166,7 @@
       <c r="B14" s="24">
         <v>12</v>
       </c>
-      <c r="C14" s="94" t="s">
+      <c r="C14" s="97" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="30" t="s">
@@ -29180,7 +29180,7 @@
       <c r="B15" s="24">
         <v>13</v>
       </c>
-      <c r="C15" s="94"/>
+      <c r="C15" s="97"/>
       <c r="D15" s="30" t="s">
         <v>13</v>
       </c>
@@ -29192,7 +29192,7 @@
       <c r="B16" s="24">
         <v>14</v>
       </c>
-      <c r="C16" s="94"/>
+      <c r="C16" s="97"/>
       <c r="D16" s="30" t="s">
         <v>11</v>
       </c>
@@ -29204,7 +29204,7 @@
       <c r="B17" s="24">
         <v>15</v>
       </c>
-      <c r="C17" s="94"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="30" t="s">
         <v>10</v>
       </c>
@@ -29216,7 +29216,7 @@
       <c r="B18" s="24">
         <v>16</v>
       </c>
-      <c r="C18" s="94"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="30" t="s">
         <v>43</v>
       </c>
@@ -29228,7 +29228,7 @@
       <c r="B19" s="24">
         <v>17</v>
       </c>
-      <c r="C19" s="95"/>
+      <c r="C19" s="98"/>
       <c r="D19" s="30" t="s">
         <v>8</v>
       </c>
@@ -29240,7 +29240,7 @@
       <c r="B20" s="31">
         <v>18</v>
       </c>
-      <c r="C20" s="96" t="s">
+      <c r="C20" s="99" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="32" t="s">
@@ -29254,7 +29254,7 @@
       <c r="B21" s="34">
         <v>19</v>
       </c>
-      <c r="C21" s="97"/>
+      <c r="C21" s="100"/>
       <c r="D21" s="35" t="s">
         <v>6</v>
       </c>
@@ -29266,7 +29266,7 @@
       <c r="B22" s="31">
         <v>20</v>
       </c>
-      <c r="C22" s="96" t="s">
+      <c r="C22" s="99" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="36" t="s">
@@ -29280,7 +29280,7 @@
       <c r="B23" s="34">
         <v>21</v>
       </c>
-      <c r="C23" s="98"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="36" t="s">
         <v>4</v>
       </c>
@@ -29292,7 +29292,7 @@
       <c r="B24" s="31">
         <v>22</v>
       </c>
-      <c r="C24" s="97"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="37" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
update energy calibration baseline
</commit_message>
<xml_diff>
--- a/data/database/DATA_Enerdata_input ThreeMe.xlsx
+++ b/data/database/DATA_Enerdata_input ThreeMe.xlsx
@@ -73,8 +73,8 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
-    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="2" r:id="rId10"/>
+    <pivotCache cacheId="3" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1110,6 +1110,15 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
@@ -1263,13 +1272,7 @@
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -1387,9 +1390,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -3707,7 +3707,146 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item x="4"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="22">
+        <item x="0"/>
+        <item x="10"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="8"/>
+        <item x="19"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item x="18"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="1"/>
+        <item x="17"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="11"/>
+        <item sd="0" x="20"/>
+        <item x="16"/>
+        <item x="12"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item h="1" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="9"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Somme de 2014" fld="3" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2020" fld="4" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2025" fld="5" baseField="2" baseItem="2"/>
+    <dataField name="Somme de 2030" fld="6" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2040" fld="7" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="5"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="83">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="2" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J3:P9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -4161,13 +4300,13 @@
     <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
+    <format dxfId="94">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
     <format dxfId="93">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
     <format dxfId="92">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5">
@@ -4180,10 +4319,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4195,7 +4334,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4214,7 +4353,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4230,7 +4369,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4242,7 +4381,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4255,7 +4394,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="85">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -4264,7 +4403,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="84">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -4283,47 +4422,49 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I3:O7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
         <item sd="0" x="0"/>
         <item x="4"/>
         <item sd="0" x="1"/>
         <item sd="0" x="2"/>
         <item sd="0" x="3"/>
         <item sd="0" x="5"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="22">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="23">
         <item x="0"/>
         <item x="10"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="8"/>
+        <item x="21"/>
+        <item x="8"/>
         <item x="19"/>
         <item x="7"/>
         <item x="13"/>
         <item x="18"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
         <item x="17"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
+        <item x="5"/>
+        <item x="6"/>
         <item x="15"/>
         <item x="9"/>
         <item x="14"/>
         <item x="11"/>
-        <item sd="0" x="20"/>
+        <item x="20"/>
         <item x="16"/>
         <item x="12"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+    <pivotField showAll="0" defaultSubtotal="0">
       <items count="8">
         <item x="4"/>
         <item x="3"/>
@@ -4341,31 +4482,23 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <items count="5">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="0"/>
+        <item sd="0" x="1"/>
+        <item n="Oil&amp;Coal" h="1" sd="0" x="3"/>
+        <item n="Elec&amp;Solar" h="1" sd="0" x="4"/>
+        <item h="1" sd="0" x="0"/>
         <item h="1" x="2"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="4">
+  <rowFields count="2">
     <field x="0"/>
     <field x="1"/>
-    <field x="9"/>
-    <field x="2"/>
   </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
+  <rowItems count="4">
     <i>
       <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i>
       <x v="4"/>
@@ -4400,16 +4533,346 @@
       <x v="5"/>
     </i>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="9" hier="-1"/>
+  </pageFields>
   <dataFields count="6">
-    <dataField name="Somme de 2014" fld="3" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2020" fld="4" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2025" fld="5" baseField="2" baseItem="2"/>
-    <dataField name="Somme de 2030" fld="6" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2040" fld="7" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="5"/>
+    <dataField name="Somme de 2014" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2020" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2025" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2030" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2040" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="94">
+  <formats count="32">
+    <format dxfId="31">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="20"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="21"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -4422,8 +4885,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -4550,835 +5013,6 @@
     <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="51">
-    <format dxfId="50">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="49">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="48">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="47">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="46">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="44">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="43">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="42">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="41">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="12"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="40">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="39">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="37">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="19"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="19"/>
-          </reference>
-          <reference field="2" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="34">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="33">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="32">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="9"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="26">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="11"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="21">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="13"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="20">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="14"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="18">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="16"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="17">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="16"/>
-          </reference>
-          <reference field="2" count="5">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="15">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="20"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="14">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="20"/>
-          </reference>
-          <reference field="2" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="11">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="10">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="15"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="15"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="17"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="5">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="17"/>
-          </reference>
-          <reference field="2" count="3">
-            <x v="2"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="18"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="18"/>
-          </reference>
-          <reference field="2" count="2">
-            <x v="2"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="21"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="21"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I3:O7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item x="4"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="23">
-        <item x="0"/>
-        <item x="10"/>
-        <item x="21"/>
-        <item x="8"/>
-        <item x="19"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="18"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="17"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="11"/>
-        <item x="20"/>
-        <item x="16"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="8">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item h="1" x="5"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
-      <items count="5">
-        <item sd="0" x="1"/>
-        <item n="Oil&amp;Coal" h="1" sd="0" x="3"/>
-        <item n="Elec&amp;Solar" h="1" sd="0" x="4"/>
-        <item h="1" sd="0" x="0"/>
-        <item h="1" x="2"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="9" hier="-1"/>
-  </pageFields>
-  <dataFields count="6">
-    <dataField name="Somme de 2014" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2020" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2025" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2030" fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2040" fld="7" baseField="0" baseItem="0"/>
-    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="32">
     <format dxfId="82">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
@@ -5402,6 +5036,22 @@
     </format>
     <format dxfId="80">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="79">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
             <x v="1"/>
@@ -5409,7 +5059,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="78">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5421,7 +5071,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="77">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="76">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5433,7 +5098,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="75">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5445,7 +5125,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="73">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -5454,7 +5149,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="71">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5466,7 +5161,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="70">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5478,7 +5189,27 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="68">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="19"/>
+          </reference>
+          <reference field="2" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -5487,7 +5218,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5499,7 +5230,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="65">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5511,7 +5258,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="63">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5523,7 +5285,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="61">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5535,7 +5316,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="59">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5547,7 +5347,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="57">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5559,7 +5378,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="55">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="11"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5571,7 +5409,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="53">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5583,7 +5440,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="51">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="14"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="50">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5595,7 +5471,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="49">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="16"/>
+          </reference>
+          <reference field="2" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="48">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -5604,7 +5499,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="47">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5616,7 +5511,27 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="46">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="20"/>
+          </reference>
+          <reference field="2" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -5625,7 +5540,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="44">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5637,7 +5552,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="43">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5649,7 +5579,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="41">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="40">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5661,7 +5607,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="39">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="15"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5673,7 +5634,24 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="37">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="17"/>
+          </reference>
+          <reference field="2" count="3">
+            <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5685,7 +5663,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="35">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="18"/>
+          </reference>
+          <reference field="2" count="2">
+            <x v="2"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5697,17 +5691,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="33">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="21"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="53">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="52">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="51">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -16566,8 +16566,8 @@
   </sheetPr>
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U22" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:AM45"/>
+    <sheetView tabSelected="1" topLeftCell="C38" workbookViewId="0">
+      <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20789,147 +20789,147 @@
       </c>
       <c r="C41" s="67">
         <f>B41+($S41-$B41)/($S$13-$B$13)</f>
-        <v>36.976427439893911</v>
+        <v>36.976665608439539</v>
       </c>
       <c r="D41" s="67">
         <f t="shared" ref="D41:R41" si="124">C41+($S41-$B41)/($S$13-$B$13)</f>
-        <v>36.924854879787823</v>
+        <v>36.92533121687908</v>
       </c>
       <c r="E41" s="67">
         <f t="shared" si="124"/>
-        <v>36.873282319681735</v>
+        <v>36.873996825318621</v>
       </c>
       <c r="F41" s="67">
         <f t="shared" si="124"/>
-        <v>36.821709759575647</v>
+        <v>36.822662433758161</v>
       </c>
       <c r="G41" s="67">
         <f t="shared" si="124"/>
-        <v>36.770137199469559</v>
+        <v>36.771328042197702</v>
       </c>
       <c r="H41" s="67">
         <f t="shared" si="124"/>
-        <v>36.718564639363471</v>
+        <v>36.719993650637242</v>
       </c>
       <c r="I41" s="67">
         <f t="shared" si="124"/>
-        <v>36.666992079257383</v>
+        <v>36.668659259076783</v>
       </c>
       <c r="J41" s="67">
         <f t="shared" si="124"/>
-        <v>36.615419519151295</v>
+        <v>36.617324867516324</v>
       </c>
       <c r="K41" s="67">
         <f t="shared" si="124"/>
-        <v>36.563846959045208</v>
+        <v>36.565990475955864</v>
       </c>
       <c r="L41" s="67">
         <f t="shared" si="124"/>
-        <v>36.51227439893912</v>
+        <v>36.514656084395405</v>
       </c>
       <c r="M41" s="67">
         <f t="shared" si="124"/>
-        <v>36.460701838833032</v>
+        <v>36.463321692834946</v>
       </c>
       <c r="N41" s="67">
         <f t="shared" si="124"/>
-        <v>36.409129278726944</v>
+        <v>36.411987301274486</v>
       </c>
       <c r="O41" s="67">
         <f t="shared" si="124"/>
-        <v>36.357556718620856</v>
+        <v>36.360652909714027</v>
       </c>
       <c r="P41" s="67">
         <f t="shared" si="124"/>
-        <v>36.305984158514768</v>
+        <v>36.309318518153567</v>
       </c>
       <c r="Q41" s="67">
         <f t="shared" si="124"/>
-        <v>36.25441159840868</v>
+        <v>36.257984126593108</v>
       </c>
       <c r="R41" s="67">
         <f t="shared" si="124"/>
-        <v>36.202839038302592</v>
+        <v>36.206649735032649</v>
       </c>
       <c r="S41" s="76">
-        <f>AB4</f>
-        <v>36.151266478196455</v>
+        <f>AC4</f>
+        <v>36.155315343472189</v>
       </c>
       <c r="T41" s="67">
         <f>S41+($AM41-$S41)/($AM$13-$S$13)</f>
-        <v>36.152223907297554</v>
+        <v>36.1560703293095</v>
       </c>
       <c r="U41" s="67">
         <f t="shared" ref="U41:AL41" si="125">T41+($AM41-$S41)/($AM$13-$S$13)</f>
-        <v>36.153181336398653</v>
+        <v>36.156825315146818</v>
       </c>
       <c r="V41" s="67">
         <f t="shared" si="125"/>
-        <v>36.154138765499752</v>
+        <v>36.157580300984137</v>
       </c>
       <c r="W41" s="67">
         <f t="shared" si="125"/>
-        <v>36.155096194600851</v>
+        <v>36.158335286821455</v>
       </c>
       <c r="X41" s="67">
         <f t="shared" si="125"/>
-        <v>36.156053623701951</v>
+        <v>36.159090272658773</v>
       </c>
       <c r="Y41" s="67">
         <f t="shared" si="125"/>
-        <v>36.15701105280305</v>
+        <v>36.159845258496091</v>
       </c>
       <c r="Z41" s="67">
         <f t="shared" si="125"/>
-        <v>36.157968481904149</v>
+        <v>36.160600244333409</v>
       </c>
       <c r="AA41" s="67">
         <f t="shared" si="125"/>
-        <v>36.158925911005248</v>
+        <v>36.161355230170727</v>
       </c>
       <c r="AB41" s="67">
         <f t="shared" si="125"/>
-        <v>36.159883340106347</v>
+        <v>36.162110216008045</v>
       </c>
       <c r="AC41" s="67">
         <f t="shared" si="125"/>
-        <v>36.160840769207446</v>
+        <v>36.162865201845364</v>
       </c>
       <c r="AD41" s="67">
         <f t="shared" si="125"/>
-        <v>36.161798198308546</v>
+        <v>36.163620187682682</v>
       </c>
       <c r="AE41" s="67">
         <f t="shared" si="125"/>
-        <v>36.162755627409645</v>
+        <v>36.16437517352</v>
       </c>
       <c r="AF41" s="67">
         <f t="shared" si="125"/>
-        <v>36.163713056510744</v>
+        <v>36.165130159357318</v>
       </c>
       <c r="AG41" s="67">
         <f t="shared" si="125"/>
-        <v>36.164670485611843</v>
+        <v>36.165885145194636</v>
       </c>
       <c r="AH41" s="67">
         <f t="shared" si="125"/>
-        <v>36.165627914712942</v>
+        <v>36.166640131031954</v>
       </c>
       <c r="AI41" s="67">
         <f t="shared" si="125"/>
-        <v>36.166585343814042</v>
+        <v>36.167395116869272</v>
       </c>
       <c r="AJ41" s="67">
         <f t="shared" si="125"/>
-        <v>36.167542772915141</v>
+        <v>36.168150102706591</v>
       </c>
       <c r="AK41" s="67">
         <f t="shared" si="125"/>
-        <v>36.16850020201624</v>
+        <v>36.168905088543909</v>
       </c>
       <c r="AL41" s="67">
         <f t="shared" si="125"/>
-        <v>36.169457631117339</v>
+        <v>36.169660074381227</v>
       </c>
       <c r="AM41" s="76">
         <f>AE4</f>
@@ -20945,147 +20945,147 @@
       </c>
       <c r="C42" s="67">
         <f t="shared" ref="C42:R42" si="126">B42+($S42-$B42)/($S$13-$B$13)</f>
-        <v>556.92640345564723</v>
+        <v>566.14729290436208</v>
       </c>
       <c r="D42" s="67">
         <f t="shared" si="126"/>
-        <v>582.86880691129443</v>
+        <v>601.31058580872411</v>
       </c>
       <c r="E42" s="67">
         <f t="shared" si="126"/>
-        <v>608.81121036694162</v>
+        <v>636.47387871308615</v>
       </c>
       <c r="F42" s="67">
         <f t="shared" si="126"/>
-        <v>634.75361382258882</v>
+        <v>671.63717161744819</v>
       </c>
       <c r="G42" s="67">
         <f t="shared" si="126"/>
-        <v>660.69601727823601</v>
+        <v>706.80046452181023</v>
       </c>
       <c r="H42" s="67">
         <f t="shared" si="126"/>
-        <v>686.63842073388321</v>
+        <v>741.96375742617226</v>
       </c>
       <c r="I42" s="67">
         <f t="shared" si="126"/>
-        <v>712.5808241895304</v>
+        <v>777.1270503305343</v>
       </c>
       <c r="J42" s="67">
         <f t="shared" si="126"/>
-        <v>738.5232276451776</v>
+        <v>812.29034323489634</v>
       </c>
       <c r="K42" s="67">
         <f t="shared" si="126"/>
-        <v>764.46563110082479</v>
+        <v>847.45363613925838</v>
       </c>
       <c r="L42" s="67">
         <f t="shared" si="126"/>
-        <v>790.40803455647199</v>
+        <v>882.61692904362042</v>
       </c>
       <c r="M42" s="67">
         <f t="shared" si="126"/>
-        <v>816.35043801211918</v>
+        <v>917.78022194798245</v>
       </c>
       <c r="N42" s="67">
         <f t="shared" si="126"/>
-        <v>842.29284146776638</v>
+        <v>952.94351485234449</v>
       </c>
       <c r="O42" s="67">
         <f t="shared" si="126"/>
-        <v>868.23524492341357</v>
+        <v>988.10680775670653</v>
       </c>
       <c r="P42" s="67">
         <f t="shared" si="126"/>
-        <v>894.17764837906077</v>
+        <v>1023.2701006610686</v>
       </c>
       <c r="Q42" s="67">
         <f t="shared" si="126"/>
-        <v>920.12005183470797</v>
+        <v>1058.4333935654306</v>
       </c>
       <c r="R42" s="67">
         <f t="shared" si="126"/>
-        <v>946.06245529035516</v>
+        <v>1093.5966864697928</v>
       </c>
       <c r="S42" s="76">
-        <f t="shared" ref="S42:S45" si="127">AB5</f>
-        <v>972.00485874600304</v>
+        <f t="shared" ref="S42:S45" si="127">AC5</f>
+        <v>1128.7599793741551</v>
       </c>
       <c r="T42" s="67">
         <f t="shared" ref="T42:AL42" si="128">S42+($AM42-$S42)/($AM$13-$S$13)</f>
-        <v>1009.3250493729497</v>
+        <v>1158.2424139696941</v>
       </c>
       <c r="U42" s="67">
         <f t="shared" si="128"/>
-        <v>1046.6452399998964</v>
+        <v>1187.7248485652331</v>
       </c>
       <c r="V42" s="67">
         <f t="shared" si="128"/>
-        <v>1083.965430626843</v>
+        <v>1217.207283160772</v>
       </c>
       <c r="W42" s="67">
         <f t="shared" si="128"/>
-        <v>1121.2856212537897</v>
+        <v>1246.689717756311</v>
       </c>
       <c r="X42" s="67">
         <f t="shared" si="128"/>
-        <v>1158.6058118807364</v>
+        <v>1276.1721523518499</v>
       </c>
       <c r="Y42" s="67">
         <f t="shared" si="128"/>
-        <v>1195.9260025076831</v>
+        <v>1305.6545869473889</v>
       </c>
       <c r="Z42" s="67">
         <f t="shared" si="128"/>
-        <v>1233.2461931346297</v>
+        <v>1335.1370215429279</v>
       </c>
       <c r="AA42" s="67">
         <f t="shared" si="128"/>
-        <v>1270.5663837615764</v>
+        <v>1364.6194561384668</v>
       </c>
       <c r="AB42" s="67">
         <f t="shared" si="128"/>
-        <v>1307.8865743885231</v>
+        <v>1394.1018907340058</v>
       </c>
       <c r="AC42" s="67">
         <f t="shared" si="128"/>
-        <v>1345.2067650154697</v>
+        <v>1423.5843253295448</v>
       </c>
       <c r="AD42" s="67">
         <f t="shared" si="128"/>
-        <v>1382.5269556424164</v>
+        <v>1453.0667599250837</v>
       </c>
       <c r="AE42" s="67">
         <f t="shared" si="128"/>
-        <v>1419.8471462693631</v>
+        <v>1482.5491945206227</v>
       </c>
       <c r="AF42" s="67">
         <f t="shared" si="128"/>
-        <v>1457.1673368963097</v>
+        <v>1512.0316291161616</v>
       </c>
       <c r="AG42" s="67">
         <f t="shared" si="128"/>
-        <v>1494.4875275232564</v>
+        <v>1541.5140637117006</v>
       </c>
       <c r="AH42" s="67">
         <f t="shared" si="128"/>
-        <v>1531.8077181502031</v>
+        <v>1570.9964983072396</v>
       </c>
       <c r="AI42" s="67">
         <f t="shared" si="128"/>
-        <v>1569.1279087771497</v>
+        <v>1600.4789329027785</v>
       </c>
       <c r="AJ42" s="67">
         <f t="shared" si="128"/>
-        <v>1606.4480994040964</v>
+        <v>1629.9613674983175</v>
       </c>
       <c r="AK42" s="67">
         <f t="shared" si="128"/>
-        <v>1643.7682900310431</v>
+        <v>1659.4438020938564</v>
       </c>
       <c r="AL42" s="67">
         <f t="shared" si="128"/>
-        <v>1681.0884806579897</v>
+        <v>1688.9262366893954</v>
       </c>
       <c r="AM42" s="76">
         <f t="shared" ref="AM42:AM45" si="129">AE5</f>
@@ -21101,147 +21101,147 @@
       </c>
       <c r="C43" s="67">
         <f t="shared" ref="C43:R43" si="130">B43+($S43-$B43)/($S$13-$B$13)</f>
-        <v>4.3718944010850418</v>
+        <v>4.4609751374703599</v>
       </c>
       <c r="D43" s="67">
         <f t="shared" si="130"/>
-        <v>4.562331409170084</v>
+        <v>4.7404928819407193</v>
       </c>
       <c r="E43" s="67">
         <f t="shared" si="130"/>
-        <v>4.7527684172551261</v>
+        <v>5.0200106264110786</v>
       </c>
       <c r="F43" s="67">
         <f t="shared" si="130"/>
-        <v>4.9432054253401683</v>
+        <v>5.299528370881438</v>
       </c>
       <c r="G43" s="67">
         <f t="shared" si="130"/>
-        <v>5.1336424334252104</v>
+        <v>5.5790461153517974</v>
       </c>
       <c r="H43" s="67">
         <f t="shared" si="130"/>
-        <v>5.3240794415102526</v>
+        <v>5.8585638598221568</v>
       </c>
       <c r="I43" s="67">
         <f t="shared" si="130"/>
-        <v>5.5145164495952947</v>
+        <v>6.1380816042925161</v>
       </c>
       <c r="J43" s="67">
         <f t="shared" si="130"/>
-        <v>5.7049534576803369</v>
+        <v>6.4175993487628755</v>
       </c>
       <c r="K43" s="67">
         <f t="shared" si="130"/>
-        <v>5.8953904657653791</v>
+        <v>6.6971170932332349</v>
       </c>
       <c r="L43" s="67">
         <f t="shared" si="130"/>
-        <v>6.0858274738504212</v>
+        <v>6.9766348377035943</v>
       </c>
       <c r="M43" s="67">
         <f t="shared" si="130"/>
-        <v>6.2762644819354634</v>
+        <v>7.2561525821739536</v>
       </c>
       <c r="N43" s="67">
         <f t="shared" si="130"/>
-        <v>6.4667014900205055</v>
+        <v>7.535670326644313</v>
       </c>
       <c r="O43" s="67">
         <f t="shared" si="130"/>
-        <v>6.6571384981055477</v>
+        <v>7.8151880711146724</v>
       </c>
       <c r="P43" s="67">
         <f t="shared" si="130"/>
-        <v>6.8475755061905899</v>
+        <v>8.0947058155850318</v>
       </c>
       <c r="Q43" s="67">
         <f t="shared" si="130"/>
-        <v>7.038012514275632</v>
+        <v>8.3742235600553911</v>
       </c>
       <c r="R43" s="67">
         <f t="shared" si="130"/>
-        <v>7.2284495223606742</v>
+        <v>8.6537413045257505</v>
       </c>
       <c r="S43" s="76">
         <f t="shared" si="127"/>
-        <v>7.4188865304457199</v>
+        <v>8.933259048996117</v>
       </c>
       <c r="T43" s="67">
         <f t="shared" ref="T43:AL43" si="131">S43+($AM43-$S43)/($AM$13-$S$13)</f>
-        <v>7.8568705951971927</v>
+        <v>9.2955244878200709</v>
       </c>
       <c r="U43" s="67">
         <f t="shared" si="131"/>
-        <v>8.2948546599486654</v>
+        <v>9.6577899266440248</v>
       </c>
       <c r="V43" s="67">
         <f t="shared" si="131"/>
-        <v>8.7328387247001391</v>
+        <v>10.020055365467979</v>
       </c>
       <c r="W43" s="67">
         <f t="shared" si="131"/>
-        <v>9.1708227894516128</v>
+        <v>10.382320804291933</v>
       </c>
       <c r="X43" s="67">
         <f t="shared" si="131"/>
-        <v>9.6088068542030864</v>
+        <v>10.744586243115887</v>
       </c>
       <c r="Y43" s="67">
         <f t="shared" si="131"/>
-        <v>10.04679091895456</v>
+        <v>11.10685168193984</v>
       </c>
       <c r="Z43" s="67">
         <f t="shared" si="131"/>
-        <v>10.484774983706034</v>
+        <v>11.469117120763794</v>
       </c>
       <c r="AA43" s="67">
         <f t="shared" si="131"/>
-        <v>10.922759048457507</v>
+        <v>11.831382559587748</v>
       </c>
       <c r="AB43" s="67">
         <f t="shared" si="131"/>
-        <v>11.360743113208981</v>
+        <v>12.193647998411702</v>
       </c>
       <c r="AC43" s="67">
         <f t="shared" si="131"/>
-        <v>11.798727177960455</v>
+        <v>12.555913437235656</v>
       </c>
       <c r="AD43" s="67">
         <f t="shared" si="131"/>
-        <v>12.236711242711928</v>
+        <v>12.91817887605961</v>
       </c>
       <c r="AE43" s="67">
         <f t="shared" si="131"/>
-        <v>12.674695307463402</v>
+        <v>13.280444314883564</v>
       </c>
       <c r="AF43" s="67">
         <f t="shared" si="131"/>
-        <v>13.112679372214876</v>
+        <v>13.642709753707518</v>
       </c>
       <c r="AG43" s="67">
         <f t="shared" si="131"/>
-        <v>13.550663436966349</v>
+        <v>14.004975192531472</v>
       </c>
       <c r="AH43" s="67">
         <f t="shared" si="131"/>
-        <v>13.988647501717823</v>
+        <v>14.367240631355426</v>
       </c>
       <c r="AI43" s="67">
         <f t="shared" si="131"/>
-        <v>14.426631566469297</v>
+        <v>14.729506070179379</v>
       </c>
       <c r="AJ43" s="67">
         <f t="shared" si="131"/>
-        <v>14.86461563122077</v>
+        <v>15.091771509003333</v>
       </c>
       <c r="AK43" s="67">
         <f t="shared" si="131"/>
-        <v>15.302599695972244</v>
+        <v>15.454036947827287</v>
       </c>
       <c r="AL43" s="67">
         <f t="shared" si="131"/>
-        <v>15.740583760723718</v>
+        <v>15.816302386651241</v>
       </c>
       <c r="AM43" s="76">
         <f t="shared" si="129"/>
@@ -21257,147 +21257,147 @@
       </c>
       <c r="C44" s="67">
         <f t="shared" ref="C44:R44" si="132">B44+($S44-$B44)/($S$13-$B$13)</f>
-        <v>89.813130897632774</v>
+        <v>90.455222487882551</v>
       </c>
       <c r="D44" s="67">
         <f t="shared" si="132"/>
-        <v>93.299262155265552</v>
+        <v>94.583445335765106</v>
       </c>
       <c r="E44" s="67">
         <f t="shared" si="132"/>
-        <v>96.78539341289833</v>
+        <v>98.71166818364766</v>
       </c>
       <c r="F44" s="67">
         <f t="shared" si="132"/>
-        <v>100.27152467053111</v>
+        <v>102.83989103153021</v>
       </c>
       <c r="G44" s="67">
         <f t="shared" si="132"/>
-        <v>103.75765592816389</v>
+        <v>106.96811387941277</v>
       </c>
       <c r="H44" s="67">
         <f t="shared" si="132"/>
-        <v>107.24378718579666</v>
+        <v>111.09633672729532</v>
       </c>
       <c r="I44" s="67">
         <f t="shared" si="132"/>
-        <v>110.72991844342944</v>
+        <v>115.22455957517788</v>
       </c>
       <c r="J44" s="67">
         <f t="shared" si="132"/>
-        <v>114.21604970106222</v>
+        <v>119.35278242306043</v>
       </c>
       <c r="K44" s="67">
         <f t="shared" si="132"/>
-        <v>117.702180958695</v>
+        <v>123.48100527094299</v>
       </c>
       <c r="L44" s="67">
         <f t="shared" si="132"/>
-        <v>121.18831221632777</v>
+        <v>127.60922811882554</v>
       </c>
       <c r="M44" s="67">
         <f t="shared" si="132"/>
-        <v>124.67444347396055</v>
+        <v>131.73745096670808</v>
       </c>
       <c r="N44" s="67">
         <f t="shared" si="132"/>
-        <v>128.16057473159333</v>
+        <v>135.86567381459062</v>
       </c>
       <c r="O44" s="67">
         <f t="shared" si="132"/>
-        <v>131.64670598922612</v>
+        <v>139.99389666247316</v>
       </c>
       <c r="P44" s="67">
         <f t="shared" si="132"/>
-        <v>135.13283724685891</v>
+        <v>144.1221195103557</v>
       </c>
       <c r="Q44" s="67">
         <f t="shared" si="132"/>
-        <v>138.6189685044917</v>
+        <v>148.25034235823824</v>
       </c>
       <c r="R44" s="67">
         <f t="shared" si="132"/>
-        <v>142.1050997621245</v>
+        <v>152.37856520612078</v>
       </c>
       <c r="S44" s="76">
         <f t="shared" si="127"/>
-        <v>145.59123101975723</v>
+        <v>156.50678805400332</v>
       </c>
       <c r="T44" s="67">
         <f t="shared" ref="T44:AL44" si="133">S44+($AM44-$S44)/($AM$13-$S$13)</f>
-        <v>147.96048327394132</v>
+        <v>158.33026245647511</v>
       </c>
       <c r="U44" s="67">
         <f t="shared" si="133"/>
-        <v>150.32973552812541</v>
+        <v>160.1537368589469</v>
       </c>
       <c r="V44" s="67">
         <f t="shared" si="133"/>
-        <v>152.6989877823095</v>
+        <v>161.97721126141869</v>
       </c>
       <c r="W44" s="67">
         <f t="shared" si="133"/>
-        <v>155.06824003649359</v>
+        <v>163.80068566389048</v>
       </c>
       <c r="X44" s="67">
         <f t="shared" si="133"/>
-        <v>157.43749229067768</v>
+        <v>165.62416006636226</v>
       </c>
       <c r="Y44" s="67">
         <f t="shared" si="133"/>
-        <v>159.80674454486177</v>
+        <v>167.44763446883405</v>
       </c>
       <c r="Z44" s="67">
         <f t="shared" si="133"/>
-        <v>162.17599679904586</v>
+        <v>169.27110887130584</v>
       </c>
       <c r="AA44" s="67">
         <f t="shared" si="133"/>
-        <v>164.54524905322995</v>
+        <v>171.09458327377763</v>
       </c>
       <c r="AB44" s="67">
         <f t="shared" si="133"/>
-        <v>166.91450130741404</v>
+        <v>172.91805767624942</v>
       </c>
       <c r="AC44" s="67">
         <f t="shared" si="133"/>
-        <v>169.28375356159813</v>
+        <v>174.74153207872121</v>
       </c>
       <c r="AD44" s="67">
         <f t="shared" si="133"/>
-        <v>171.65300581578222</v>
+        <v>176.565006481193</v>
       </c>
       <c r="AE44" s="67">
         <f t="shared" si="133"/>
-        <v>174.02225806996631</v>
+        <v>178.38848088366478</v>
       </c>
       <c r="AF44" s="67">
         <f t="shared" si="133"/>
-        <v>176.3915103241504</v>
+        <v>180.21195528613657</v>
       </c>
       <c r="AG44" s="67">
         <f t="shared" si="133"/>
-        <v>178.76076257833449</v>
+        <v>182.03542968860836</v>
       </c>
       <c r="AH44" s="67">
         <f t="shared" si="133"/>
-        <v>181.13001483251858</v>
+        <v>183.85890409108015</v>
       </c>
       <c r="AI44" s="67">
         <f t="shared" si="133"/>
-        <v>183.49926708670267</v>
+        <v>185.68237849355194</v>
       </c>
       <c r="AJ44" s="67">
         <f t="shared" si="133"/>
-        <v>185.86851934088676</v>
+        <v>187.50585289602373</v>
       </c>
       <c r="AK44" s="67">
         <f t="shared" si="133"/>
-        <v>188.23777159507085</v>
+        <v>189.32932729849551</v>
       </c>
       <c r="AL44" s="67">
         <f t="shared" si="133"/>
-        <v>190.60702384925494</v>
+        <v>191.1528017009673</v>
       </c>
       <c r="AM44" s="76">
         <f t="shared" si="129"/>
@@ -21413,147 +21413,147 @@
       </c>
       <c r="C45" s="67">
         <f t="shared" ref="C45:R45" si="134">B45+($S45-$B45)/($S$13-$B$13)</f>
-        <v>206.81768014679571</v>
+        <v>210.68904891176064</v>
       </c>
       <c r="D45" s="67">
         <f t="shared" si="134"/>
-        <v>218.41481769359143</v>
+        <v>226.15755522352129</v>
       </c>
       <c r="E45" s="67">
         <f t="shared" si="134"/>
-        <v>230.01195524038715</v>
+        <v>241.62606153528193</v>
       </c>
       <c r="F45" s="67">
         <f t="shared" si="134"/>
-        <v>241.60909278718287</v>
+        <v>257.09456784704258</v>
       </c>
       <c r="G45" s="67">
         <f t="shared" si="134"/>
-        <v>253.2062303339786</v>
+        <v>272.56307415880326</v>
       </c>
       <c r="H45" s="67">
         <f t="shared" si="134"/>
-        <v>264.80336788077432</v>
+        <v>288.03158047056394</v>
       </c>
       <c r="I45" s="67">
         <f t="shared" si="134"/>
-        <v>276.40050542757001</v>
+        <v>303.50008678232462</v>
       </c>
       <c r="J45" s="67">
         <f t="shared" si="134"/>
-        <v>287.9976429743657</v>
+        <v>318.96859309408529</v>
       </c>
       <c r="K45" s="67">
         <f t="shared" si="134"/>
-        <v>299.5947805211614</v>
+        <v>334.43709940584597</v>
       </c>
       <c r="L45" s="67">
         <f t="shared" si="134"/>
-        <v>311.19191806795709</v>
+        <v>349.90560571760665</v>
       </c>
       <c r="M45" s="67">
         <f t="shared" si="134"/>
-        <v>322.78905561475278</v>
+        <v>365.37411202936732</v>
       </c>
       <c r="N45" s="67">
         <f t="shared" si="134"/>
-        <v>334.38619316154848</v>
+        <v>380.842618341128</v>
       </c>
       <c r="O45" s="67">
         <f t="shared" si="134"/>
-        <v>345.98333070834417</v>
+        <v>396.31112465288868</v>
       </c>
       <c r="P45" s="67">
         <f t="shared" si="134"/>
-        <v>357.58046825513986</v>
+        <v>411.77963096464936</v>
       </c>
       <c r="Q45" s="67">
         <f t="shared" si="134"/>
-        <v>369.17760580193556</v>
+        <v>427.24813727641003</v>
       </c>
       <c r="R45" s="67">
         <f t="shared" si="134"/>
-        <v>380.77474334873125</v>
+        <v>442.71664358817071</v>
       </c>
       <c r="S45" s="76">
         <f t="shared" si="127"/>
-        <v>392.37188089552723</v>
+        <v>458.18514989993105</v>
       </c>
       <c r="T45" s="67">
         <f t="shared" ref="T45:AL45" si="135">S45+($AM45-$S45)/($AM$13-$S$13)</f>
-        <v>406.57880398317337</v>
+        <v>469.10140953735703</v>
       </c>
       <c r="U45" s="67">
         <f t="shared" si="135"/>
-        <v>420.78572707081952</v>
+        <v>480.01766917478301</v>
       </c>
       <c r="V45" s="67">
         <f t="shared" si="135"/>
-        <v>434.99265015846566</v>
+        <v>490.93392881220899</v>
       </c>
       <c r="W45" s="67">
         <f t="shared" si="135"/>
-        <v>449.19957324611181</v>
+        <v>501.85018844963497</v>
       </c>
       <c r="X45" s="67">
         <f t="shared" si="135"/>
-        <v>463.40649633375796</v>
+        <v>512.76644808706089</v>
       </c>
       <c r="Y45" s="67">
         <f t="shared" si="135"/>
-        <v>477.6134194214041</v>
+        <v>523.68270772448682</v>
       </c>
       <c r="Z45" s="67">
         <f t="shared" si="135"/>
-        <v>491.82034250905025</v>
+        <v>534.59896736191274</v>
       </c>
       <c r="AA45" s="67">
         <f t="shared" si="135"/>
-        <v>506.0272655966964</v>
+        <v>545.51522699933867</v>
       </c>
       <c r="AB45" s="67">
         <f t="shared" si="135"/>
-        <v>520.2341886843426</v>
+        <v>556.43148663676459</v>
       </c>
       <c r="AC45" s="67">
         <f t="shared" si="135"/>
-        <v>534.44111177198874</v>
+        <v>567.34774627419051</v>
       </c>
       <c r="AD45" s="67">
         <f t="shared" si="135"/>
-        <v>548.64803485963489</v>
+        <v>578.26400591161644</v>
       </c>
       <c r="AE45" s="67">
         <f t="shared" si="135"/>
-        <v>562.85495794728104</v>
+        <v>589.18026554904236</v>
       </c>
       <c r="AF45" s="67">
         <f t="shared" si="135"/>
-        <v>577.06188103492718</v>
+        <v>600.09652518646828</v>
       </c>
       <c r="AG45" s="67">
         <f t="shared" si="135"/>
-        <v>591.26880412257333</v>
+        <v>611.01278482389421</v>
       </c>
       <c r="AH45" s="67">
         <f t="shared" si="135"/>
-        <v>605.47572721021947</v>
+        <v>621.92904446132013</v>
       </c>
       <c r="AI45" s="67">
         <f t="shared" si="135"/>
-        <v>619.68265029786562</v>
+        <v>632.84530409874606</v>
       </c>
       <c r="AJ45" s="67">
         <f t="shared" si="135"/>
-        <v>633.88957338551177</v>
+        <v>643.76156373617198</v>
       </c>
       <c r="AK45" s="67">
         <f t="shared" si="135"/>
-        <v>648.09649647315791</v>
+        <v>654.6778233735979</v>
       </c>
       <c r="AL45" s="67">
         <f t="shared" si="135"/>
-        <v>662.30341956080406</v>
+        <v>665.59408301102383</v>
       </c>
       <c r="AM45" s="76">
         <f t="shared" si="129"/>
@@ -21570,147 +21570,147 @@
       </c>
       <c r="C46" s="69">
         <f t="shared" ref="C46" si="136">SUM(C41:C45)</f>
-        <v>894.90553634105459</v>
+        <v>908.72920504991521</v>
       </c>
       <c r="D46" s="69">
         <f t="shared" ref="D46" si="137">SUM(D41:D45)</f>
-        <v>936.07007304910928</v>
+        <v>963.71741046683019</v>
       </c>
       <c r="E46" s="69">
         <f t="shared" ref="E46" si="138">SUM(E41:E45)</f>
-        <v>977.23460975716387</v>
+        <v>1018.7056158837455</v>
       </c>
       <c r="F46" s="69">
         <f t="shared" ref="F46" si="139">SUM(F41:F45)</f>
-        <v>1018.3991464652186</v>
+        <v>1073.6938213006606</v>
       </c>
       <c r="G46" s="69">
         <f t="shared" ref="G46" si="140">SUM(G41:G45)</f>
-        <v>1059.5636831732731</v>
+        <v>1128.6820267175758</v>
       </c>
       <c r="H46" s="69">
         <f t="shared" ref="H46" si="141">SUM(H41:H45)</f>
-        <v>1100.7282198813277</v>
+        <v>1183.670232134491</v>
       </c>
       <c r="I46" s="69">
         <f t="shared" ref="I46" si="142">SUM(I41:I45)</f>
-        <v>1141.8927565893825</v>
+        <v>1238.6584375514062</v>
       </c>
       <c r="J46" s="69">
         <f t="shared" ref="J46" si="143">SUM(J41:J45)</f>
-        <v>1183.0572932974369</v>
+        <v>1293.6466429683212</v>
       </c>
       <c r="K46" s="69">
         <f t="shared" ref="K46" si="144">SUM(K41:K45)</f>
-        <v>1224.2218300054917</v>
+        <v>1348.6348483852366</v>
       </c>
       <c r="L46" s="69">
         <f t="shared" ref="L46" si="145">SUM(L41:L45)</f>
-        <v>1265.3863667135463</v>
+        <v>1403.6230538021516</v>
       </c>
       <c r="M46" s="69">
         <f t="shared" ref="M46" si="146">SUM(M41:M45)</f>
-        <v>1306.5509034216011</v>
+        <v>1458.6112592190668</v>
       </c>
       <c r="N46" s="69">
         <f t="shared" ref="N46" si="147">SUM(N41:N45)</f>
-        <v>1347.7154401296557</v>
+        <v>1513.5994646359818</v>
       </c>
       <c r="O46" s="69">
         <f t="shared" ref="O46" si="148">SUM(O41:O45)</f>
-        <v>1388.8799768377103</v>
+        <v>1568.587670052897</v>
       </c>
       <c r="P46" s="69">
         <f t="shared" ref="P46" si="149">SUM(P41:P45)</f>
-        <v>1430.0445135457649</v>
+        <v>1623.5758754698124</v>
       </c>
       <c r="Q46" s="69">
         <f t="shared" ref="Q46" si="150">SUM(Q41:Q45)</f>
-        <v>1471.2090502538194</v>
+        <v>1678.5640808867274</v>
       </c>
       <c r="R46" s="69">
         <f t="shared" ref="R46" si="151">SUM(R41:R45)</f>
-        <v>1512.373586961874</v>
+        <v>1733.5522863036426</v>
       </c>
       <c r="S46" s="79">
         <f t="shared" ref="S46" si="152">SUM(S41:S45)</f>
-        <v>1553.5381236699297</v>
+        <v>1788.5404917205581</v>
       </c>
       <c r="T46" s="69">
         <f t="shared" ref="T46" si="153">SUM(T41:T45)</f>
-        <v>1607.8734311325593</v>
+        <v>1831.1256807806558</v>
       </c>
       <c r="U46" s="69">
         <f t="shared" ref="U46" si="154">SUM(U41:U45)</f>
-        <v>1662.2087385951886</v>
+        <v>1873.7108698407537</v>
       </c>
       <c r="V46" s="69">
         <f t="shared" ref="V46" si="155">SUM(V41:V45)</f>
-        <v>1716.5440460578182</v>
+        <v>1916.2960589008517</v>
       </c>
       <c r="W46" s="69">
         <f t="shared" ref="W46" si="156">SUM(W41:W45)</f>
-        <v>1770.8793535204477</v>
+        <v>1958.8812479609501</v>
       </c>
       <c r="X46" s="69">
         <f t="shared" ref="X46" si="157">SUM(X41:X45)</f>
-        <v>1825.2146609830772</v>
+        <v>2001.466437021048</v>
       </c>
       <c r="Y46" s="69">
         <f t="shared" ref="Y46" si="158">SUM(Y41:Y45)</f>
-        <v>1879.5499684457063</v>
+        <v>2044.0516260811457</v>
       </c>
       <c r="Z46" s="69">
         <f t="shared" ref="Z46" si="159">SUM(Z41:Z45)</f>
-        <v>1933.8852759083361</v>
+        <v>2086.6368151412435</v>
       </c>
       <c r="AA46" s="69">
         <f t="shared" ref="AA46" si="160">SUM(AA41:AA45)</f>
-        <v>1988.2205833709656</v>
+        <v>2129.2220042013419</v>
       </c>
       <c r="AB46" s="69">
         <f t="shared" ref="AB46" si="161">SUM(AB41:AB45)</f>
-        <v>2042.555890833595</v>
+        <v>2171.8071932614394</v>
       </c>
       <c r="AC46" s="69">
         <f t="shared" ref="AC46" si="162">SUM(AC41:AC45)</f>
-        <v>2096.8911982962245</v>
+        <v>2214.3923823215373</v>
       </c>
       <c r="AD46" s="69">
         <f t="shared" ref="AD46" si="163">SUM(AD41:AD45)</f>
-        <v>2151.2265057588538</v>
+        <v>2256.9775713816352</v>
       </c>
       <c r="AE46" s="69">
         <f t="shared" ref="AE46" si="164">SUM(AE41:AE45)</f>
-        <v>2205.5618132214836</v>
+        <v>2299.5627604417336</v>
       </c>
       <c r="AF46" s="69">
         <f t="shared" ref="AF46" si="165">SUM(AF41:AF45)</f>
-        <v>2259.8971206841129</v>
+        <v>2342.1479495018316</v>
       </c>
       <c r="AG46" s="69">
         <f t="shared" ref="AG46" si="166">SUM(AG41:AG45)</f>
-        <v>2314.2324281467422</v>
+        <v>2384.7331385619291</v>
       </c>
       <c r="AH46" s="69">
         <f t="shared" ref="AH46" si="167">SUM(AH41:AH45)</f>
-        <v>2368.567735609372</v>
+        <v>2427.318327622027</v>
       </c>
       <c r="AI46" s="69">
         <f t="shared" ref="AI46" si="168">SUM(AI41:AI45)</f>
-        <v>2422.9030430720013</v>
+        <v>2469.9035166821254</v>
       </c>
       <c r="AJ46" s="69">
         <f t="shared" ref="AJ46" si="169">SUM(AJ41:AJ45)</f>
-        <v>2477.2383505346306</v>
+        <v>2512.4887057422229</v>
       </c>
       <c r="AK46" s="69">
         <f t="shared" ref="AK46" si="170">SUM(AK41:AK45)</f>
-        <v>2531.5736579972604</v>
+        <v>2555.0738948023209</v>
       </c>
       <c r="AL46" s="69">
         <f t="shared" ref="AL46" si="171">SUM(AL41:AL45)</f>
-        <v>2585.9089654598902</v>
+        <v>2597.6590838624188</v>
       </c>
       <c r="AM46" s="79">
         <f t="shared" ref="AM46" si="172">SUM(AM41:AM45)</f>

</xml_diff>

<commit_message>
upadte baseline and EE scenariio
</commit_message>
<xml_diff>
--- a/data/database/DATA_Enerdata_input ThreeMe.xlsx
+++ b/data/database/DATA_Enerdata_input ThreeMe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Energy final consumption-Mtoe" sheetId="1" r:id="rId1"/>
@@ -73,8 +73,8 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId10"/>
-    <pivotCache cacheId="3" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1359,9 +1359,6 @@
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
@@ -1390,6 +1387,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="#,##0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="#,##0.0"/>
@@ -3707,146 +3707,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item sd="0" x="0"/>
-        <item x="4"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="5"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="22">
-        <item x="0"/>
-        <item x="10"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="8"/>
-        <item x="19"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="18"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="1"/>
-        <item x="17"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="11"/>
-        <item sd="0" x="20"/>
-        <item x="16"/>
-        <item x="12"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="8">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item h="1" x="5"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="0"/>
-    <field x="1"/>
-    <field x="9"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-  </colItems>
-  <dataFields count="6">
-    <dataField name="Somme de 2014" fld="3" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2020" fld="4" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2025" fld="5" baseField="2" baseItem="2"/>
-    <dataField name="Somme de 2030" fld="6" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2040" fld="7" baseField="1" baseItem="0"/>
-    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="5"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="83">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="2" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J3:P9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -4300,13 +4161,13 @@
     <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
-    <format dxfId="94">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
     <format dxfId="93">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
     <format dxfId="92">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5">
@@ -4319,10 +4180,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4334,7 +4195,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4353,7 +4214,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4369,7 +4230,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4381,7 +4242,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -4394,7 +4255,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="84">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -4403,7 +4264,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="83">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -4422,8 +4283,147 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item x="4"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="22">
+        <item x="0"/>
+        <item x="10"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="8"/>
+        <item x="19"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item x="18"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="1"/>
+        <item x="17"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="11"/>
+        <item sd="0" x="20"/>
+        <item x="16"/>
+        <item x="12"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item h="1" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="9"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Somme de 2014" fld="3" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2020" fld="4" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2025" fld="5" baseField="2" baseItem="2"/>
+    <dataField name="Somme de 2030" fld="6" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2040" fld="7" baseField="1" baseItem="0"/>
+    <dataField name="Somme de 2050" fld="8" baseField="0" baseItem="5"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="94">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I3:O7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -4886,7 +4886,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -16566,7 +16566,7 @@
   </sheetPr>
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C38" workbookViewId="0">
+    <sheetView topLeftCell="C38" workbookViewId="0">
       <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
@@ -22787,8 +22787,8 @@
   </sheetPr>
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:AI46"/>
+    <sheetView tabSelected="1" topLeftCell="AE18" workbookViewId="0">
+      <selection activeCell="AO42" sqref="AO42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27010,147 +27010,147 @@
       </c>
       <c r="C41" s="67">
         <f>B41+($S41-$B41)/($S$13-$B$13)</f>
-        <v>36.976427439893911</v>
+        <v>36.976665608439539</v>
       </c>
       <c r="D41" s="67">
         <f t="shared" ref="D41:R41" si="27">C41+($S41-$B41)/($S$13-$B$13)</f>
-        <v>36.924854879787823</v>
+        <v>36.92533121687908</v>
       </c>
       <c r="E41" s="67">
         <f t="shared" si="27"/>
-        <v>36.873282319681735</v>
+        <v>36.873996825318621</v>
       </c>
       <c r="F41" s="67">
         <f t="shared" si="27"/>
-        <v>36.821709759575647</v>
+        <v>36.822662433758161</v>
       </c>
       <c r="G41" s="67">
         <f t="shared" si="27"/>
-        <v>36.770137199469559</v>
+        <v>36.771328042197702</v>
       </c>
       <c r="H41" s="67">
         <f t="shared" si="27"/>
-        <v>36.718564639363471</v>
+        <v>36.719993650637242</v>
       </c>
       <c r="I41" s="67">
         <f t="shared" si="27"/>
-        <v>36.666992079257383</v>
+        <v>36.668659259076783</v>
       </c>
       <c r="J41" s="67">
         <f t="shared" si="27"/>
-        <v>36.615419519151295</v>
+        <v>36.617324867516324</v>
       </c>
       <c r="K41" s="67">
         <f t="shared" si="27"/>
-        <v>36.563846959045208</v>
+        <v>36.565990475955864</v>
       </c>
       <c r="L41" s="67">
         <f t="shared" si="27"/>
-        <v>36.51227439893912</v>
+        <v>36.514656084395405</v>
       </c>
       <c r="M41" s="67">
         <f t="shared" si="27"/>
-        <v>36.460701838833032</v>
+        <v>36.463321692834946</v>
       </c>
       <c r="N41" s="67">
         <f t="shared" si="27"/>
-        <v>36.409129278726944</v>
+        <v>36.411987301274486</v>
       </c>
       <c r="O41" s="67">
         <f t="shared" si="27"/>
-        <v>36.357556718620856</v>
+        <v>36.360652909714027</v>
       </c>
       <c r="P41" s="67">
         <f t="shared" si="27"/>
-        <v>36.305984158514768</v>
+        <v>36.309318518153567</v>
       </c>
       <c r="Q41" s="67">
         <f t="shared" si="27"/>
-        <v>36.25441159840868</v>
+        <v>36.257984126593108</v>
       </c>
       <c r="R41" s="67">
         <f t="shared" si="27"/>
-        <v>36.202839038302592</v>
+        <v>36.206649735032649</v>
       </c>
       <c r="S41" s="76">
-        <f>AB4</f>
-        <v>36.151266478196455</v>
+        <f>AC4</f>
+        <v>36.155315343472189</v>
       </c>
       <c r="T41" s="67">
         <f>S41+($AM41-$S41)/($AM$13-$S$13)</f>
-        <v>36.152223907297554</v>
+        <v>36.1560703293095</v>
       </c>
       <c r="U41" s="67">
         <f t="shared" ref="U41:AL41" si="28">T41+($AM41-$S41)/($AM$13-$S$13)</f>
-        <v>36.153181336398653</v>
+        <v>36.156825315146818</v>
       </c>
       <c r="V41" s="67">
         <f t="shared" si="28"/>
-        <v>36.154138765499752</v>
+        <v>36.157580300984137</v>
       </c>
       <c r="W41" s="67">
         <f t="shared" si="28"/>
-        <v>36.155096194600851</v>
+        <v>36.158335286821455</v>
       </c>
       <c r="X41" s="67">
         <f t="shared" si="28"/>
-        <v>36.156053623701951</v>
+        <v>36.159090272658773</v>
       </c>
       <c r="Y41" s="67">
         <f t="shared" si="28"/>
-        <v>36.15701105280305</v>
+        <v>36.159845258496091</v>
       </c>
       <c r="Z41" s="67">
         <f t="shared" si="28"/>
-        <v>36.157968481904149</v>
+        <v>36.160600244333409</v>
       </c>
       <c r="AA41" s="67">
         <f t="shared" si="28"/>
-        <v>36.158925911005248</v>
+        <v>36.161355230170727</v>
       </c>
       <c r="AB41" s="67">
         <f t="shared" si="28"/>
-        <v>36.159883340106347</v>
+        <v>36.162110216008045</v>
       </c>
       <c r="AC41" s="67">
         <f t="shared" si="28"/>
-        <v>36.160840769207446</v>
+        <v>36.162865201845364</v>
       </c>
       <c r="AD41" s="67">
         <f t="shared" si="28"/>
-        <v>36.161798198308546</v>
+        <v>36.163620187682682</v>
       </c>
       <c r="AE41" s="67">
         <f t="shared" si="28"/>
-        <v>36.162755627409645</v>
+        <v>36.16437517352</v>
       </c>
       <c r="AF41" s="67">
         <f t="shared" si="28"/>
-        <v>36.163713056510744</v>
+        <v>36.165130159357318</v>
       </c>
       <c r="AG41" s="67">
         <f t="shared" si="28"/>
-        <v>36.164670485611843</v>
+        <v>36.165885145194636</v>
       </c>
       <c r="AH41" s="67">
         <f t="shared" si="28"/>
-        <v>36.165627914712942</v>
+        <v>36.166640131031954</v>
       </c>
       <c r="AI41" s="67">
         <f t="shared" si="28"/>
-        <v>36.166585343814042</v>
+        <v>36.167395116869272</v>
       </c>
       <c r="AJ41" s="67">
         <f t="shared" si="28"/>
-        <v>36.167542772915141</v>
+        <v>36.168150102706591</v>
       </c>
       <c r="AK41" s="67">
         <f t="shared" si="28"/>
-        <v>36.16850020201624</v>
+        <v>36.168905088543909</v>
       </c>
       <c r="AL41" s="67">
         <f t="shared" si="28"/>
-        <v>36.169457631117339</v>
+        <v>36.169660074381227</v>
       </c>
       <c r="AM41" s="76">
         <f>AE4</f>
@@ -27166,147 +27166,147 @@
       </c>
       <c r="C42" s="67">
         <f t="shared" ref="C42:R45" si="29">B42+($S42-$B42)/($S$13-$B$13)</f>
-        <v>538.20452654105702</v>
+        <v>540.96735988378248</v>
       </c>
       <c r="D42" s="67">
         <f t="shared" si="29"/>
-        <v>545.425053082114</v>
+        <v>550.95071976756492</v>
       </c>
       <c r="E42" s="67">
         <f t="shared" si="29"/>
-        <v>552.64557962317099</v>
+        <v>560.93407965134736</v>
       </c>
       <c r="F42" s="67">
         <f t="shared" si="29"/>
-        <v>559.86610616422797</v>
+        <v>570.9174395351298</v>
       </c>
       <c r="G42" s="67">
         <f t="shared" si="29"/>
-        <v>567.08663270528496</v>
+        <v>580.90079941891224</v>
       </c>
       <c r="H42" s="67">
         <f t="shared" si="29"/>
-        <v>574.30715924634194</v>
+        <v>590.88415930269468</v>
       </c>
       <c r="I42" s="67">
         <f t="shared" si="29"/>
-        <v>581.52768578739892</v>
+        <v>600.86751918647713</v>
       </c>
       <c r="J42" s="67">
         <f t="shared" si="29"/>
-        <v>588.74821232845591</v>
+        <v>610.85087907025957</v>
       </c>
       <c r="K42" s="67">
         <f t="shared" si="29"/>
-        <v>595.96873886951289</v>
+        <v>620.83423895404201</v>
       </c>
       <c r="L42" s="67">
         <f t="shared" si="29"/>
-        <v>603.18926541056987</v>
+        <v>630.81759883782445</v>
       </c>
       <c r="M42" s="67">
         <f t="shared" si="29"/>
-        <v>610.40979195162686</v>
+        <v>640.80095872160689</v>
       </c>
       <c r="N42" s="67">
         <f t="shared" si="29"/>
-        <v>617.63031849268384</v>
+        <v>650.78431860538933</v>
       </c>
       <c r="O42" s="67">
         <f t="shared" si="29"/>
-        <v>624.85084503374082</v>
+        <v>660.76767848917177</v>
       </c>
       <c r="P42" s="67">
         <f t="shared" si="29"/>
-        <v>632.07137157479781</v>
+        <v>670.75103837295421</v>
       </c>
       <c r="Q42" s="67">
         <f t="shared" si="29"/>
-        <v>639.29189811585479</v>
+        <v>680.73439825673665</v>
       </c>
       <c r="R42" s="67">
         <f t="shared" si="29"/>
-        <v>646.51242465691178</v>
+        <v>690.71775814051909</v>
       </c>
       <c r="S42" s="76">
-        <f t="shared" ref="S42:S45" si="30">AB5</f>
-        <v>653.73295119796933</v>
+        <f t="shared" ref="S42:S45" si="30">AC5</f>
+        <v>700.70111802430188</v>
       </c>
       <c r="T42" s="67">
         <f t="shared" ref="T42:AL45" si="31">S42+($AM42-$S42)/($AM$13-$S$13)</f>
-        <v>662.87200160847567</v>
+        <v>707.49176009349162</v>
       </c>
       <c r="U42" s="67">
         <f t="shared" si="31"/>
-        <v>672.01105201898201</v>
+        <v>714.28240216268136</v>
       </c>
       <c r="V42" s="67">
         <f t="shared" si="31"/>
-        <v>681.15010242948836</v>
+        <v>721.07304423187111</v>
       </c>
       <c r="W42" s="67">
         <f t="shared" si="31"/>
-        <v>690.2891528399947</v>
+        <v>727.86368630106085</v>
       </c>
       <c r="X42" s="67">
         <f t="shared" si="31"/>
-        <v>699.42820325050104</v>
+        <v>734.6543283702506</v>
       </c>
       <c r="Y42" s="67">
         <f t="shared" si="31"/>
-        <v>708.56725366100738</v>
+        <v>741.44497043944034</v>
       </c>
       <c r="Z42" s="67">
         <f t="shared" si="31"/>
-        <v>717.70630407151373</v>
+        <v>748.23561250863008</v>
       </c>
       <c r="AA42" s="67">
         <f t="shared" si="31"/>
-        <v>726.84535448202007</v>
+        <v>755.02625457781983</v>
       </c>
       <c r="AB42" s="67">
         <f t="shared" si="31"/>
-        <v>735.98440489252641</v>
+        <v>761.81689664700957</v>
       </c>
       <c r="AC42" s="67">
         <f t="shared" si="31"/>
-        <v>745.12345530303276</v>
+        <v>768.60753871619931</v>
       </c>
       <c r="AD42" s="67">
         <f t="shared" si="31"/>
-        <v>754.2625057135391</v>
+        <v>775.39818078538906</v>
       </c>
       <c r="AE42" s="67">
         <f t="shared" si="31"/>
-        <v>763.40155612404544</v>
+        <v>782.1888228545788</v>
       </c>
       <c r="AF42" s="67">
         <f t="shared" si="31"/>
-        <v>772.54060653455178</v>
+        <v>788.97946492376855</v>
       </c>
       <c r="AG42" s="67">
         <f t="shared" si="31"/>
-        <v>781.67965694505813</v>
+        <v>795.77010699295829</v>
       </c>
       <c r="AH42" s="67">
         <f t="shared" si="31"/>
-        <v>790.81870735556447</v>
+        <v>802.56074906214803</v>
       </c>
       <c r="AI42" s="67">
         <f t="shared" si="31"/>
-        <v>799.95775776607081</v>
+        <v>809.35139113133778</v>
       </c>
       <c r="AJ42" s="67">
         <f t="shared" si="31"/>
-        <v>809.09680817657716</v>
+        <v>816.14203320052752</v>
       </c>
       <c r="AK42" s="67">
         <f t="shared" si="31"/>
-        <v>818.2358585870835</v>
+        <v>822.93267526971727</v>
       </c>
       <c r="AL42" s="67">
         <f t="shared" si="31"/>
-        <v>827.37490899758984</v>
+        <v>829.72331733890701</v>
       </c>
       <c r="AM42" s="76">
         <f t="shared" ref="AM42:AM45" si="32">AE5</f>
@@ -27322,147 +27322,147 @@
       </c>
       <c r="C43" s="67">
         <f t="shared" si="29"/>
-        <v>5.538180251651414</v>
+        <v>6.1756143176852767</v>
       </c>
       <c r="D43" s="67">
         <f t="shared" si="29"/>
-        <v>6.8949031103028284</v>
+        <v>8.1697712423705529</v>
       </c>
       <c r="E43" s="67">
         <f t="shared" si="29"/>
-        <v>8.2516259689542437</v>
+        <v>10.163928167055829</v>
       </c>
       <c r="F43" s="67">
         <f t="shared" si="29"/>
-        <v>9.6083488276056581</v>
+        <v>12.158085091741105</v>
       </c>
       <c r="G43" s="67">
         <f t="shared" si="29"/>
-        <v>10.965071686257073</v>
+        <v>14.152242016426381</v>
       </c>
       <c r="H43" s="67">
         <f t="shared" si="29"/>
-        <v>12.321794544908487</v>
+        <v>16.146398941111659</v>
       </c>
       <c r="I43" s="67">
         <f t="shared" si="29"/>
-        <v>13.678517403559901</v>
+        <v>18.140555865796937</v>
       </c>
       <c r="J43" s="67">
         <f t="shared" si="29"/>
-        <v>15.035240262211316</v>
+        <v>20.134712790482215</v>
       </c>
       <c r="K43" s="67">
         <f t="shared" si="29"/>
-        <v>16.39196312086273</v>
+        <v>22.128869715167493</v>
       </c>
       <c r="L43" s="67">
         <f t="shared" si="29"/>
-        <v>17.748685979514143</v>
+        <v>24.123026639852771</v>
       </c>
       <c r="M43" s="67">
         <f t="shared" si="29"/>
-        <v>19.105408838165559</v>
+        <v>26.117183564538049</v>
       </c>
       <c r="N43" s="67">
         <f t="shared" si="29"/>
-        <v>20.462131696816975</v>
+        <v>28.111340489223327</v>
       </c>
       <c r="O43" s="67">
         <f t="shared" si="29"/>
-        <v>21.818854555468391</v>
+        <v>30.105497413908605</v>
       </c>
       <c r="P43" s="67">
         <f t="shared" si="29"/>
-        <v>23.175577414119807</v>
+        <v>32.099654338593879</v>
       </c>
       <c r="Q43" s="67">
         <f t="shared" si="29"/>
-        <v>24.532300272771224</v>
+        <v>34.093811263279157</v>
       </c>
       <c r="R43" s="67">
         <f t="shared" si="29"/>
-        <v>25.88902313142264</v>
+        <v>36.087968187964435</v>
       </c>
       <c r="S43" s="76">
         <f t="shared" si="30"/>
-        <v>27.245745990074042</v>
+        <v>38.082125112649706</v>
       </c>
       <c r="T43" s="67">
         <f t="shared" si="31"/>
-        <v>30.580084767428968</v>
+        <v>40.87464493387585</v>
       </c>
       <c r="U43" s="67">
         <f t="shared" si="31"/>
-        <v>33.914423544783894</v>
+        <v>43.667164755101993</v>
       </c>
       <c r="V43" s="67">
         <f t="shared" si="31"/>
-        <v>37.248762322138823</v>
+        <v>46.459684576328137</v>
       </c>
       <c r="W43" s="67">
         <f t="shared" si="31"/>
-        <v>40.583101099493753</v>
+        <v>49.25220439755428</v>
       </c>
       <c r="X43" s="67">
         <f t="shared" si="31"/>
-        <v>43.917439876848682</v>
+        <v>52.044724218780424</v>
       </c>
       <c r="Y43" s="67">
         <f t="shared" si="31"/>
-        <v>47.251778654203612</v>
+        <v>54.837244040006567</v>
       </c>
       <c r="Z43" s="67">
         <f t="shared" si="31"/>
-        <v>50.586117431558542</v>
+        <v>57.629763861232711</v>
       </c>
       <c r="AA43" s="67">
         <f t="shared" si="31"/>
-        <v>53.920456208913471</v>
+        <v>60.422283682458854</v>
       </c>
       <c r="AB43" s="67">
         <f t="shared" si="31"/>
-        <v>57.254794986268401</v>
+        <v>63.214803503684998</v>
       </c>
       <c r="AC43" s="67">
         <f t="shared" si="31"/>
-        <v>60.58913376362333</v>
+        <v>66.007323324911141</v>
       </c>
       <c r="AD43" s="67">
         <f t="shared" si="31"/>
-        <v>63.92347254097826</v>
+        <v>68.799843146137292</v>
       </c>
       <c r="AE43" s="67">
         <f t="shared" si="31"/>
-        <v>67.257811318333182</v>
+        <v>71.592362967363442</v>
       </c>
       <c r="AF43" s="67">
         <f t="shared" si="31"/>
-        <v>70.592150095688112</v>
+        <v>74.384882788589593</v>
       </c>
       <c r="AG43" s="67">
         <f t="shared" si="31"/>
-        <v>73.926488873043041</v>
+        <v>77.177402609815744</v>
       </c>
       <c r="AH43" s="67">
         <f t="shared" si="31"/>
-        <v>77.260827650397971</v>
+        <v>79.969922431041894</v>
       </c>
       <c r="AI43" s="67">
         <f t="shared" si="31"/>
-        <v>80.595166427752901</v>
+        <v>82.762442252268045</v>
       </c>
       <c r="AJ43" s="67">
         <f t="shared" si="31"/>
-        <v>83.92950520510783</v>
+        <v>85.554962073494195</v>
       </c>
       <c r="AK43" s="67">
         <f t="shared" si="31"/>
-        <v>87.26384398246276</v>
+        <v>88.347481894720346</v>
       </c>
       <c r="AL43" s="67">
         <f t="shared" si="31"/>
-        <v>90.598182759817689</v>
+        <v>91.140001715946497</v>
       </c>
       <c r="AM43" s="76">
         <f t="shared" si="32"/>
@@ -27478,147 +27478,147 @@
       </c>
       <c r="C44" s="67">
         <f t="shared" si="29"/>
-        <v>86.038919844671994</v>
+        <v>85.460687333948314</v>
       </c>
       <c r="D44" s="67">
         <f t="shared" si="29"/>
-        <v>85.750840049343992</v>
+        <v>84.594375027896632</v>
       </c>
       <c r="E44" s="67">
         <f t="shared" si="29"/>
-        <v>85.46276025401599</v>
+        <v>83.72806272184495</v>
       </c>
       <c r="F44" s="67">
         <f t="shared" si="29"/>
-        <v>85.174680458687988</v>
+        <v>82.861750415793267</v>
       </c>
       <c r="G44" s="67">
         <f t="shared" si="29"/>
-        <v>84.886600663359985</v>
+        <v>81.995438109741585</v>
       </c>
       <c r="H44" s="67">
         <f t="shared" si="29"/>
-        <v>84.598520868031983</v>
+        <v>81.129125803689902</v>
       </c>
       <c r="I44" s="67">
         <f t="shared" si="29"/>
-        <v>84.310441072703981</v>
+        <v>80.26281349763822</v>
       </c>
       <c r="J44" s="67">
         <f t="shared" si="29"/>
-        <v>84.022361277375978</v>
+        <v>79.396501191586538</v>
       </c>
       <c r="K44" s="67">
         <f t="shared" si="29"/>
-        <v>83.734281482047976</v>
+        <v>78.530188885534855</v>
       </c>
       <c r="L44" s="67">
         <f t="shared" si="29"/>
-        <v>83.446201686719974</v>
+        <v>77.663876579483173</v>
       </c>
       <c r="M44" s="67">
         <f t="shared" si="29"/>
-        <v>83.158121891391971</v>
+        <v>76.79756427343149</v>
       </c>
       <c r="N44" s="67">
         <f t="shared" si="29"/>
-        <v>82.870042096063969</v>
+        <v>75.931251967379808</v>
       </c>
       <c r="O44" s="67">
         <f t="shared" si="29"/>
-        <v>82.581962300735967</v>
+        <v>75.064939661328125</v>
       </c>
       <c r="P44" s="67">
         <f t="shared" si="29"/>
-        <v>82.293882505407964</v>
+        <v>74.198627355276443</v>
       </c>
       <c r="Q44" s="67">
         <f t="shared" si="29"/>
-        <v>82.005802710079962</v>
+        <v>73.332315049224761</v>
       </c>
       <c r="R44" s="67">
         <f t="shared" si="29"/>
-        <v>81.71772291475196</v>
+        <v>72.466002743173078</v>
       </c>
       <c r="S44" s="76">
         <f t="shared" si="30"/>
-        <v>81.429643119423957</v>
+        <v>71.599690437121282</v>
       </c>
       <c r="T44" s="67">
         <f t="shared" si="31"/>
-        <v>80.122814188639438</v>
+        <v>70.784359140451897</v>
       </c>
       <c r="U44" s="67">
         <f t="shared" si="31"/>
-        <v>78.815985257854919</v>
+        <v>69.969027843782513</v>
       </c>
       <c r="V44" s="67">
         <f t="shared" si="31"/>
-        <v>77.5091563270704</v>
+        <v>69.153696547113128</v>
       </c>
       <c r="W44" s="67">
         <f t="shared" si="31"/>
-        <v>76.202327396285881</v>
+        <v>68.338365250443744</v>
       </c>
       <c r="X44" s="67">
         <f t="shared" si="31"/>
-        <v>74.895498465501362</v>
+        <v>67.523033953774359</v>
       </c>
       <c r="Y44" s="67">
         <f t="shared" si="31"/>
-        <v>73.588669534716843</v>
+        <v>66.707702657104974</v>
       </c>
       <c r="Z44" s="67">
         <f t="shared" si="31"/>
-        <v>72.281840603932324</v>
+        <v>65.89237136043559</v>
       </c>
       <c r="AA44" s="67">
         <f t="shared" si="31"/>
-        <v>70.975011673147804</v>
+        <v>65.077040063766205</v>
       </c>
       <c r="AB44" s="67">
         <f t="shared" si="31"/>
-        <v>69.668182742363285</v>
+        <v>64.26170876709682</v>
       </c>
       <c r="AC44" s="67">
         <f t="shared" si="31"/>
-        <v>68.361353811578766</v>
+        <v>63.446377470427443</v>
       </c>
       <c r="AD44" s="67">
         <f t="shared" si="31"/>
-        <v>67.054524880794247</v>
+        <v>62.631046173758065</v>
       </c>
       <c r="AE44" s="67">
         <f t="shared" si="31"/>
-        <v>65.747695950009728</v>
+        <v>61.815714877088688</v>
       </c>
       <c r="AF44" s="67">
         <f t="shared" si="31"/>
-        <v>64.440867019225209</v>
+        <v>61.00038358041931</v>
       </c>
       <c r="AG44" s="67">
         <f t="shared" si="31"/>
-        <v>63.134038088440697</v>
+        <v>60.185052283749933</v>
       </c>
       <c r="AH44" s="67">
         <f t="shared" si="31"/>
-        <v>61.827209157656185</v>
+        <v>59.369720987080555</v>
       </c>
       <c r="AI44" s="67">
         <f t="shared" si="31"/>
-        <v>60.520380226871673</v>
+        <v>58.554389690411178</v>
       </c>
       <c r="AJ44" s="67">
         <f t="shared" si="31"/>
-        <v>59.213551296087161</v>
+        <v>57.7390583937418</v>
       </c>
       <c r="AK44" s="67">
         <f t="shared" si="31"/>
-        <v>57.906722365302649</v>
+        <v>56.923727097072423</v>
       </c>
       <c r="AL44" s="67">
         <f t="shared" si="31"/>
-        <v>56.599893434518137</v>
+        <v>56.108395800403045</v>
       </c>
       <c r="AM44" s="76">
         <f t="shared" si="32"/>
@@ -27634,147 +27634,147 @@
       </c>
       <c r="C45" s="67">
         <f t="shared" si="29"/>
-        <v>201.5750545588854</v>
+        <v>203.58966615226362</v>
       </c>
       <c r="D45" s="67">
         <f t="shared" si="29"/>
-        <v>207.92956651777081</v>
+        <v>211.95878970452725</v>
       </c>
       <c r="E45" s="67">
         <f t="shared" si="29"/>
-        <v>214.28407847665622</v>
+        <v>220.32791325679088</v>
       </c>
       <c r="F45" s="67">
         <f t="shared" si="29"/>
-        <v>220.63859043554163</v>
+        <v>228.69703680905451</v>
       </c>
       <c r="G45" s="67">
         <f t="shared" si="29"/>
-        <v>226.99310239442704</v>
+        <v>237.06616036131814</v>
       </c>
       <c r="H45" s="67">
         <f t="shared" si="29"/>
-        <v>233.34761435331245</v>
+        <v>245.43528391358177</v>
       </c>
       <c r="I45" s="67">
         <f t="shared" si="29"/>
-        <v>239.70212631219786</v>
+        <v>253.8044074658454</v>
       </c>
       <c r="J45" s="67">
         <f t="shared" si="29"/>
-        <v>246.05663827108327</v>
+        <v>262.17353101810903</v>
       </c>
       <c r="K45" s="67">
         <f t="shared" si="29"/>
-        <v>252.41115022996868</v>
+        <v>270.54265457037269</v>
       </c>
       <c r="L45" s="67">
         <f t="shared" si="29"/>
-        <v>258.76566218885409</v>
+        <v>278.91177812263635</v>
       </c>
       <c r="M45" s="67">
         <f t="shared" si="29"/>
-        <v>265.12017414773948</v>
+        <v>287.28090167490001</v>
       </c>
       <c r="N45" s="67">
         <f t="shared" si="29"/>
-        <v>271.47468610662486</v>
+        <v>295.65002522716367</v>
       </c>
       <c r="O45" s="67">
         <f t="shared" si="29"/>
-        <v>277.82919806551024</v>
+        <v>304.01914877942733</v>
       </c>
       <c r="P45" s="67">
         <f t="shared" si="29"/>
-        <v>284.18371002439562</v>
+        <v>312.38827233169098</v>
       </c>
       <c r="Q45" s="67">
         <f t="shared" si="29"/>
-        <v>290.53822198328101</v>
+        <v>320.75739588395464</v>
       </c>
       <c r="R45" s="67">
         <f t="shared" si="29"/>
-        <v>296.89273394216639</v>
+        <v>329.1265194362183</v>
       </c>
       <c r="S45" s="76">
         <f t="shared" si="30"/>
-        <v>303.24724590105177</v>
+        <v>337.49564298848179</v>
       </c>
       <c r="T45" s="67">
         <f t="shared" si="31"/>
-        <v>309.20773111957686</v>
+        <v>341.74370835263539</v>
       </c>
       <c r="U45" s="67">
         <f t="shared" si="31"/>
-        <v>315.16821633810196</v>
+        <v>345.991773716789</v>
       </c>
       <c r="V45" s="67">
         <f t="shared" si="31"/>
-        <v>321.12870155662705</v>
+        <v>350.2398390809426</v>
       </c>
       <c r="W45" s="67">
         <f t="shared" si="31"/>
-        <v>327.08918677515214</v>
+        <v>354.48790444509621</v>
       </c>
       <c r="X45" s="67">
         <f t="shared" si="31"/>
-        <v>333.04967199367724</v>
+        <v>358.73596980924981</v>
       </c>
       <c r="Y45" s="67">
         <f t="shared" si="31"/>
-        <v>339.01015721220233</v>
+        <v>362.98403517340341</v>
       </c>
       <c r="Z45" s="67">
         <f t="shared" si="31"/>
-        <v>344.97064243072742</v>
+        <v>367.23210053755702</v>
       </c>
       <c r="AA45" s="67">
         <f t="shared" si="31"/>
-        <v>350.93112764925252</v>
+        <v>371.48016590171062</v>
       </c>
       <c r="AB45" s="67">
         <f t="shared" si="31"/>
-        <v>356.89161286777761</v>
+        <v>375.72823126586422</v>
       </c>
       <c r="AC45" s="67">
         <f t="shared" si="31"/>
-        <v>362.8520980863027</v>
+        <v>379.97629663001783</v>
       </c>
       <c r="AD45" s="67">
         <f t="shared" si="31"/>
-        <v>368.8125833048278</v>
+        <v>384.22436199417143</v>
       </c>
       <c r="AE45" s="67">
         <f t="shared" si="31"/>
-        <v>374.77306852335289</v>
+        <v>388.47242735832504</v>
       </c>
       <c r="AF45" s="67">
         <f t="shared" si="31"/>
-        <v>380.73355374187798</v>
+        <v>392.72049272247864</v>
       </c>
       <c r="AG45" s="67">
         <f t="shared" si="31"/>
-        <v>386.69403896040308</v>
+        <v>396.96855808663224</v>
       </c>
       <c r="AH45" s="67">
         <f t="shared" si="31"/>
-        <v>392.65452417892817</v>
+        <v>401.21662345078585</v>
       </c>
       <c r="AI45" s="67">
         <f t="shared" si="31"/>
-        <v>398.61500939745326</v>
+        <v>405.46468881493945</v>
       </c>
       <c r="AJ45" s="67">
         <f t="shared" si="31"/>
-        <v>404.57549461597836</v>
+        <v>409.71275417909305</v>
       </c>
       <c r="AK45" s="67">
         <f t="shared" si="31"/>
-        <v>410.53597983450345</v>
+        <v>413.96081954324666</v>
       </c>
       <c r="AL45" s="67">
         <f t="shared" si="31"/>
-        <v>416.49646505302854</v>
+        <v>418.20888490740026</v>
       </c>
       <c r="AM45" s="76">
         <f t="shared" si="32"/>
@@ -27791,147 +27791,147 @@
       </c>
       <c r="C46" s="69">
         <f t="shared" ref="C46:AM46" si="33">SUM(C41:C45)</f>
-        <v>868.33310863615975</v>
+        <v>873.16999329611917</v>
       </c>
       <c r="D46" s="69">
         <f t="shared" si="33"/>
-        <v>882.9252176393195</v>
+        <v>892.59898695923835</v>
       </c>
       <c r="E46" s="69">
         <f t="shared" si="33"/>
-        <v>897.51732664247913</v>
+        <v>912.02798062235763</v>
       </c>
       <c r="F46" s="69">
         <f t="shared" si="33"/>
-        <v>912.109435645639</v>
+        <v>931.45697428547692</v>
       </c>
       <c r="G46" s="69">
         <f t="shared" si="33"/>
-        <v>926.70154464879863</v>
+        <v>950.88596794859609</v>
       </c>
       <c r="H46" s="69">
         <f t="shared" si="33"/>
-        <v>941.29365365195827</v>
+        <v>970.31496161171526</v>
       </c>
       <c r="I46" s="69">
         <f t="shared" si="33"/>
-        <v>955.88576265511801</v>
+        <v>989.74395527483455</v>
       </c>
       <c r="J46" s="69">
         <f t="shared" si="33"/>
-        <v>970.47787165827776</v>
+        <v>1009.1729489379538</v>
       </c>
       <c r="K46" s="69">
         <f t="shared" si="33"/>
-        <v>985.06998066143763</v>
+        <v>1028.601942601073</v>
       </c>
       <c r="L46" s="69">
         <f t="shared" si="33"/>
-        <v>999.66208966459715</v>
+        <v>1048.0309362641922</v>
       </c>
       <c r="M46" s="69">
         <f t="shared" si="33"/>
-        <v>1014.2541986677569</v>
+        <v>1067.4599299273114</v>
       </c>
       <c r="N46" s="69">
         <f t="shared" si="33"/>
-        <v>1028.8463076709165</v>
+        <v>1086.8889235904307</v>
       </c>
       <c r="O46" s="69">
         <f t="shared" si="33"/>
-        <v>1043.4384166740763</v>
+        <v>1106.3179172535499</v>
       </c>
       <c r="P46" s="69">
         <f t="shared" si="33"/>
-        <v>1058.030525677236</v>
+        <v>1125.7469109166691</v>
       </c>
       <c r="Q46" s="69">
         <f t="shared" si="33"/>
-        <v>1072.6226346803955</v>
+        <v>1145.1759045797883</v>
       </c>
       <c r="R46" s="69">
         <f t="shared" si="33"/>
-        <v>1087.2147436835553</v>
+        <v>1164.6048982429077</v>
       </c>
       <c r="S46" s="79">
         <f t="shared" si="33"/>
-        <v>1101.8068526867155</v>
+        <v>1184.0338919060268</v>
       </c>
       <c r="T46" s="69">
         <f t="shared" si="33"/>
-        <v>1118.9348555914185</v>
+        <v>1197.0505428497643</v>
       </c>
       <c r="U46" s="69">
         <f t="shared" si="33"/>
-        <v>1136.0628584961214</v>
+        <v>1210.0671937935017</v>
       </c>
       <c r="V46" s="69">
         <f t="shared" si="33"/>
-        <v>1153.1908614008244</v>
+        <v>1223.0838447372391</v>
       </c>
       <c r="W46" s="69">
         <f t="shared" si="33"/>
-        <v>1170.3188643055273</v>
+        <v>1236.1004956809766</v>
       </c>
       <c r="X46" s="69">
         <f t="shared" si="33"/>
-        <v>1187.4468672102303</v>
+        <v>1249.117146624714</v>
       </c>
       <c r="Y46" s="69">
         <f t="shared" si="33"/>
-        <v>1204.5748701149332</v>
+        <v>1262.1337975684514</v>
       </c>
       <c r="Z46" s="69">
         <f t="shared" si="33"/>
-        <v>1221.7028730196362</v>
+        <v>1275.1504485121889</v>
       </c>
       <c r="AA46" s="69">
         <f t="shared" si="33"/>
-        <v>1238.8308759243391</v>
+        <v>1288.1670994559263</v>
       </c>
       <c r="AB46" s="69">
         <f t="shared" si="33"/>
-        <v>1255.9588788290421</v>
+        <v>1301.1837503996635</v>
       </c>
       <c r="AC46" s="69">
         <f t="shared" si="33"/>
-        <v>1273.086881733745</v>
+        <v>1314.2004013434012</v>
       </c>
       <c r="AD46" s="69">
         <f t="shared" si="33"/>
-        <v>1290.214884638448</v>
+        <v>1327.2170522871384</v>
       </c>
       <c r="AE46" s="69">
         <f t="shared" si="33"/>
-        <v>1307.3428875431509</v>
+        <v>1340.233703230876</v>
       </c>
       <c r="AF46" s="69">
         <f t="shared" si="33"/>
-        <v>1324.4708904478539</v>
+        <v>1353.2503541746134</v>
       </c>
       <c r="AG46" s="69">
         <f t="shared" si="33"/>
-        <v>1341.5988933525568</v>
+        <v>1366.2670051183509</v>
       </c>
       <c r="AH46" s="69">
         <f t="shared" si="33"/>
-        <v>1358.7268962572596</v>
+        <v>1379.2836560620883</v>
       </c>
       <c r="AI46" s="69">
         <f t="shared" si="33"/>
-        <v>1375.8548991619627</v>
+        <v>1392.3003070058257</v>
       </c>
       <c r="AJ46" s="69">
         <f t="shared" si="33"/>
-        <v>1392.9829020666657</v>
+        <v>1405.3169579495632</v>
       </c>
       <c r="AK46" s="69">
         <f t="shared" si="33"/>
-        <v>1410.1109049713687</v>
+        <v>1418.3336088933006</v>
       </c>
       <c r="AL46" s="69">
         <f t="shared" si="33"/>
-        <v>1427.2389078760716</v>
+        <v>1431.350259837038</v>
       </c>
       <c r="AM46" s="79">
         <f t="shared" si="33"/>

</xml_diff>